<commit_message>
[expression] - [`[EXCEL(...) => csvWithHeader`]: convert a contiguous cell range (from Excel worksheet) to a [`CSV`] where the first range is treated as header. - [`[EXCEL(...) => json(firstRowAsHeader)`]: convert a contiguous cell range (from Excel worksheet) to a [`JSON`] where the first range may be treated as header to impact the output JSON structure.
### [excel commands]
- [`csv(file,worksheet,range,output)`]: **NEW** command to convert a contiguous cell range (from Excel worksheet) to a CSV file (`output`).
- [`json(file,worksheet,range,header,output)`]: **NEW** command to convert a contiguous cell range (from Excel worksheet) to a JSON file (`output`).

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/demo1/artifact/script/InjestData.xlsx
+++ b/demo1/artifact/script/InjestData.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr documentId="13_ncr:1_{CA8AB993-2A9B-8C43-8543-A6241A53824D}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32"/>
   <bookViews>
-    <workbookView activeTab="1" tabRatio="500" windowHeight="25160" windowWidth="40960" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="440" firstSheet="1"/>
+    <workbookView activeTab="1" firstSheet="1" tabRatio="500" windowHeight="25160" windowWidth="40960" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="440"/>
   </bookViews>
   <sheets>
     <sheet name="#system" r:id="rId1" sheetId="4" state="hidden"/>
@@ -25,12 +25,12 @@
     <definedName name="date">'#system'!$C$2:$C$14</definedName>
     <definedName name="db">'#system'!$D$2:$D$5</definedName>
     <definedName name="desktop">'#system'!$E$2:$E$92</definedName>
-    <definedName name="excel">'#system'!$F$2:$F$8</definedName>
+    <definedName name="excel">'#system'!$F$2:$F$10</definedName>
     <definedName name="external">'#system'!$G$2:$G$3</definedName>
     <definedName name="image">'#system'!$H$2:$H$5</definedName>
     <definedName name="io">'#system'!$I$2:$I$22</definedName>
     <definedName name="jms">'#system'!$J$2:$J$4</definedName>
-    <definedName name="json">'#system'!$K$2:$K$13</definedName>
+    <definedName name="json">'#system'!$K$2:$K$14</definedName>
     <definedName name="mail">'#system'!$L$2:$L$2</definedName>
     <definedName name="math">'#system'!$K$2:$K$13</definedName>
     <definedName name="mq">'#system'!$J$2:$J$3</definedName>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1097" uniqueCount="523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1555" uniqueCount="525">
   <si>
     <t>description</t>
   </si>
@@ -1639,6 +1639,12 @@
   </si>
   <si>
     <t>put(url,body,output)</t>
+  </si>
+  <si>
+    <t>csv(file,worksheet,range,header,output)</t>
+  </si>
+  <si>
+    <t>json(file,worksheet,range,header,output)</t>
   </si>
 </sst>
 </file>
@@ -1646,7 +1652,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="43" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1831,8 +1837,102 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="823C3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="32">
+  <fills count="59">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2010,8 +2110,161 @@
         <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="34">
+  <borders count="62">
     <border>
       <left/>
       <right/>
@@ -2368,6 +2621,288 @@
         <color rgb="C3C3C3"/>
       </bottom>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
@@ -2375,7 +2910,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="74">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="2" fontId="7" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -2532,49 +3067,94 @@
     <xf applyAlignment="1" applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="13" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="13" fillId="7" fontId="13" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="17" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="17" fillId="10" fontId="15" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="21" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="21" fillId="13" fontId="16" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="16" fontId="18" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="25" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="25" fillId="19" fontId="20" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="29" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="29" fillId="22" fontId="21" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="33" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="33" fillId="25" fontId="22" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="33" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="33" fillId="25" fontId="23" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="28" fontId="24" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="31" fontId="25" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="28" fontId="26" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="41" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="37" borderId="45" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="40" borderId="49" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="43" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="46" borderId="53" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="49" borderId="57" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="52" borderId="61" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="52" borderId="61" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="55" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="58" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="55" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2961,7 +3541,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA114"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" tabSelected="false">
+    <sheetView tabSelected="false" workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
@@ -3147,7 +3727,7 @@
         <v>87</v>
       </c>
       <c r="F3" t="s">
-        <v>329</v>
+        <v>523</v>
       </c>
       <c r="G3" t="s">
         <v>28</v>
@@ -3221,7 +3801,7 @@
         <v>388</v>
       </c>
       <c r="F4" t="s">
-        <v>330</v>
+        <v>524</v>
       </c>
       <c r="H4" t="s">
         <v>352</v>
@@ -3292,7 +3872,7 @@
         <v>337</v>
       </c>
       <c r="F5" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="H5" t="s">
         <v>349</v>
@@ -3354,7 +3934,7 @@
         <v>389</v>
       </c>
       <c r="F6" t="s">
-        <v>324</v>
+        <v>330</v>
       </c>
       <c r="I6" t="s">
         <v>16</v>
@@ -3410,13 +3990,13 @@
         <v>367</v>
       </c>
       <c r="F7" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="I7" t="s">
         <v>79</v>
       </c>
       <c r="K7" t="s">
-        <v>34</v>
+        <v>316</v>
       </c>
       <c r="M7" t="s">
         <v>33</v>
@@ -3466,13 +4046,13 @@
         <v>368</v>
       </c>
       <c r="F8" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="I8" t="s">
         <v>38</v>
       </c>
       <c r="K8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M8" t="s">
         <v>90</v>
@@ -3518,11 +4098,14 @@
       <c r="E9" t="s">
         <v>307</v>
       </c>
+      <c r="F9" t="s">
+        <v>325</v>
+      </c>
       <c r="I9" t="s">
         <v>391</v>
       </c>
       <c r="K9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M9" t="s">
         <v>91</v>
@@ -3556,11 +4139,14 @@
       <c r="E10" t="s">
         <v>353</v>
       </c>
+      <c r="F10" t="s">
+        <v>326</v>
+      </c>
       <c r="I10" t="s">
         <v>17</v>
       </c>
       <c r="K10" t="s">
-        <v>497</v>
+        <v>36</v>
       </c>
       <c r="M10" t="s">
         <v>501</v>
@@ -3595,7 +4181,7 @@
         <v>42</v>
       </c>
       <c r="K11" t="s">
-        <v>39</v>
+        <v>497</v>
       </c>
       <c r="M11" t="s">
         <v>92</v>
@@ -3627,7 +4213,7 @@
         <v>80</v>
       </c>
       <c r="K12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M12" t="s">
         <v>41</v>
@@ -3656,7 +4242,7 @@
         <v>81</v>
       </c>
       <c r="K13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M13" t="s">
         <v>93</v>
@@ -3683,6 +4269,9 @@
       </c>
       <c r="I14" t="s">
         <v>82</v>
+      </c>
+      <c r="K14" t="s">
+        <v>43</v>
       </c>
       <c r="M14" t="s">
         <v>94</v>
@@ -4572,7 +5161,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P984"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" tabSelected="true">
+    <sheetView tabSelected="true" workbookViewId="0" zoomScale="100">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A5" ySplit="4"/>
       <selection activeCell="A5" pane="bottomLeft" sqref="A5"/>
     </sheetView>
@@ -15812,7 +16401,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2309A12F-BAB4-2449-A1A4-931DAD6BB5D5}">
   <dimension ref="A1:P996"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" tabSelected="false">
+    <sheetView tabSelected="false" workbookViewId="0" zoomScale="100">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A5" ySplit="4"/>
       <selection activeCell="A5" pane="bottomLeft" sqref="A5"/>
     </sheetView>

</xml_diff>

<commit_message>
- fixed failed unit tests - minor output text tweaks.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/demo1/artifact/script/InjestData.xlsx
+++ b/demo1/artifact/script/InjestData.xlsx
@@ -20,36 +20,37 @@
   </sheets>
   <definedNames>
     <definedName name="aws.s3">'#system'!$B$2:$B$9</definedName>
-    <definedName name="base">'#system'!$C$2:$C$33</definedName>
-    <definedName name="csv">'#system'!$D$2:$D$5</definedName>
+    <definedName name="base">'#system'!$D$2:$D$36</definedName>
+    <definedName name="csv">'#system'!$E$2:$E$5</definedName>
     <definedName name="date">'#system'!$C$2:$C$14</definedName>
     <definedName name="db">'#system'!$D$2:$D$5</definedName>
-    <definedName name="desktop">'#system'!$E$2:$E$92</definedName>
-    <definedName name="excel">'#system'!$F$2:$F$10</definedName>
-    <definedName name="external">'#system'!$G$2:$G$3</definedName>
-    <definedName name="image">'#system'!$H$2:$H$5</definedName>
-    <definedName name="io">'#system'!$I$2:$I$22</definedName>
-    <definedName name="jms">'#system'!$J$2:$J$4</definedName>
-    <definedName name="json">'#system'!$K$2:$K$14</definedName>
-    <definedName name="mail">'#system'!$L$2:$L$2</definedName>
+    <definedName name="desktop">'#system'!$F$2:$F$92</definedName>
+    <definedName name="excel">'#system'!$G$2:$G$14</definedName>
+    <definedName name="external">'#system'!$H$2:$H$3</definedName>
+    <definedName name="image">'#system'!$I$2:$I$6</definedName>
+    <definedName name="io">'#system'!$J$2:$J$24</definedName>
+    <definedName name="jms">'#system'!$K$2:$K$4</definedName>
+    <definedName name="json">'#system'!$L$2:$L$14</definedName>
+    <definedName name="mail">'#system'!$M$2:$M$2</definedName>
     <definedName name="math">'#system'!$K$2:$K$13</definedName>
     <definedName name="mq">'#system'!$J$2:$J$3</definedName>
     <definedName name="nextgen">'#system'!$K$2:$K$28</definedName>
-    <definedName name="number">'#system'!$M$2:$M$15</definedName>
-    <definedName name="pdf">'#system'!$N$2:$N$16</definedName>
-    <definedName name="rdbms">'#system'!$O$2:$O$7</definedName>
-    <definedName name="redis">'#system'!$P$2:$P$10</definedName>
-    <definedName name="ssh">'#system'!$S$2:$S$9</definedName>
-    <definedName name="step">'#system'!$T$2:$T$4</definedName>
-    <definedName name="target">'#system'!$A$2:$A$26</definedName>
-    <definedName name="web">'#system'!$U$2:$U$114</definedName>
-    <definedName name="webalert">'#system'!$V$2:$V$8</definedName>
-    <definedName name="webcookie">'#system'!$W$2:$W$8</definedName>
-    <definedName name="ws">'#system'!$X$2:$X$16</definedName>
-    <definedName name="xml">'#system'!$Z$2:$Z$11</definedName>
-    <definedName name="sms">'#system'!$Q$2:$Q$2</definedName>
-    <definedName name="sound">'#system'!$R$2:$R$5</definedName>
-    <definedName name="ws.async">'#system'!$Y$2:$Y$8</definedName>
+    <definedName name="number">'#system'!$N$2:$N$15</definedName>
+    <definedName name="pdf">'#system'!$O$2:$O$16</definedName>
+    <definedName name="rdbms">'#system'!$P$2:$P$7</definedName>
+    <definedName name="redis">'#system'!$Q$2:$Q$10</definedName>
+    <definedName name="ssh">'#system'!$T$2:$T$9</definedName>
+    <definedName name="step">'#system'!$U$2:$U$4</definedName>
+    <definedName name="target">'#system'!$A$2:$A$27</definedName>
+    <definedName name="web">'#system'!$V$2:$V$118</definedName>
+    <definedName name="webalert">'#system'!$W$2:$W$8</definedName>
+    <definedName name="webcookie">'#system'!$X$2:$X$8</definedName>
+    <definedName name="ws">'#system'!$Y$2:$Y$17</definedName>
+    <definedName name="xml">'#system'!$AA$2:$AA$11</definedName>
+    <definedName name="sms">'#system'!$R$2:$R$2</definedName>
+    <definedName name="sound">'#system'!$S$2:$S$5</definedName>
+    <definedName name="ws.async">'#system'!$Z$2:$Z$8</definedName>
+    <definedName name="aws.ses">'#system'!$C$2:$C$3</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
@@ -69,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1555" uniqueCount="525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2509" uniqueCount="544">
   <si>
     <t>description</t>
   </si>
@@ -1645,6 +1646,63 @@
   </si>
   <si>
     <t>json(file,worksheet,range,header,output)</t>
+  </si>
+  <si>
+    <t>aws.ses</t>
+  </si>
+  <si>
+    <t>sendHtmlMail(profile,to,subject,body)</t>
+  </si>
+  <si>
+    <t>sendTextMail(profile,to,subject,body)</t>
+  </si>
+  <si>
+    <t>assertArrayContain(array,expected)</t>
+  </si>
+  <si>
+    <t>assertArrayNotContain(array,unexpected)</t>
+  </si>
+  <si>
+    <t>saveCount(text,regex,saveVar)</t>
+  </si>
+  <si>
+    <t>assertPassword(file)</t>
+  </si>
+  <si>
+    <t>clearPassword(file,password)</t>
+  </si>
+  <si>
+    <t>columnarCsv(file,worksheet,ranges,output)</t>
+  </si>
+  <si>
+    <t>csv(file,worksheet,range,output)</t>
+  </si>
+  <si>
+    <t>setPassword(file,password)</t>
+  </si>
+  <si>
+    <t>colorbit(source,bit,saveTo)</t>
+  </si>
+  <si>
+    <t>base64(var,file)</t>
+  </si>
+  <si>
+    <t>rename(target,newName)</t>
+  </si>
+  <si>
+    <t>clickWithKeys(locator,keys)</t>
+  </si>
+  <si>
+    <t>deselect(locator,text)</t>
+  </si>
+  <si>
+    <t>openHttpBasic(url,username,password)</t>
+  </si>
+  <si>
+    <t>saveDivsAsCsv(headers,rows,cells,nextPage,file)</t>
+  </si>
+  <si>
+    <t>upload(url,body,fileParams,var)</t>
   </si>
 </sst>
 </file>
@@ -1652,7 +1710,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="43" x14ac:knownFonts="1">
+  <fonts count="75" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1931,8 +1989,210 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="823C3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="823C3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="59">
+  <fills count="113">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2263,8 +2523,314 @@
         <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="62">
+  <borders count="118">
     <border>
       <left/>
       <right/>
@@ -2903,6 +3469,570 @@
         <color rgb="C3C3C3"/>
       </bottom>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
@@ -2910,7 +4040,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="106">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="2" fontId="7" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -3112,49 +4242,145 @@
     <xf applyFont="true" borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="34" borderId="41" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="41" fillId="34" fontId="28" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="29" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="37" borderId="45" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="45" fillId="37" fontId="30" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="40" borderId="49" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="49" fillId="40" fontId="31" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="32" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="43" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="43" fontId="33" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="34" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="46" borderId="53" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="53" fillId="46" fontId="35" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="49" borderId="57" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="57" fillId="49" fontId="36" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="52" borderId="61" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="61" fillId="52" fontId="37" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="52" borderId="61" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="61" fillId="52" fontId="38" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="55" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="55" fontId="39" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="58" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="58" fontId="40" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="55" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="55" fontId="41" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="42" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="69" fillId="61" fontId="43" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="44" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="73" fillId="64" fontId="45" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="77" fillId="67" fontId="46" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="77" fillId="70" fontId="47" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="48" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="73" fontId="49" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="50" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="81" fillId="76" fontId="51" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="85" fillId="79" fontId="52" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="89" fillId="82" fontId="53" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="89" fillId="82" fontId="54" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="70" fontId="55" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="85" fontId="56" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="70" fontId="57" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="58" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="88" borderId="97" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="91" borderId="101" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="94" borderId="105" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="97" borderId="105" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="100" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="67" fillId="103" borderId="109" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="68" fillId="106" borderId="113" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="69" fillId="109" borderId="117" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="70" fillId="109" borderId="117" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="71" fillId="97" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="112" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="73" fillId="97" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -3539,7 +4765,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA114"/>
+  <dimension ref="A1:AB118"/>
   <sheetViews>
     <sheetView tabSelected="false" workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125">
       <selection activeCell="A19" sqref="A19"/>
@@ -3558,75 +4784,78 @@
         <v>372</v>
       </c>
       <c r="C1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>50</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>22</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>23</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>348</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>14</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>334</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>24</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>196</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>51</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>240</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>52</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>397</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>488</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>489</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>358</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>398</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>53</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>54</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>55</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>56</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>490</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>228</v>
       </c>
     </row>
@@ -3638,1517 +4867,1579 @@
         <v>373</v>
       </c>
       <c r="C2" t="s">
+        <v>526</v>
+      </c>
+      <c r="D2" t="s">
         <v>57</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>71</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>73</v>
       </c>
-      <c r="F2" t="s">
-        <v>48</v>
-      </c>
       <c r="G2" t="s">
+        <v>531</v>
+      </c>
+      <c r="H2" t="s">
         <v>78</v>
       </c>
-      <c r="H2" t="s">
-        <v>350</v>
-      </c>
       <c r="I2" t="s">
+        <v>536</v>
+      </c>
+      <c r="J2" t="s">
         <v>316</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>385</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>496</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>498</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>499</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>254</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>218</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>399</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>503</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>504</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>382</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>408</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>96</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>171</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>176</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>183</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>517</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>525</v>
       </c>
       <c r="B3" t="s">
         <v>374</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>527</v>
       </c>
       <c r="D3" t="s">
+        <v>528</v>
+      </c>
+      <c r="E3" t="s">
         <v>366</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>87</v>
       </c>
-      <c r="F3" t="s">
-        <v>523</v>
-      </c>
       <c r="G3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" t="s">
         <v>28</v>
       </c>
-      <c r="H3" t="s">
-        <v>351</v>
-      </c>
       <c r="I3" t="s">
+        <v>350</v>
+      </c>
+      <c r="J3" t="s">
         <v>342</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>335</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>85</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>500</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>241</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>219</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>400</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>505</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>383</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>409</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>97</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>172</v>
       </c>
-      <c r="W3" t="s">
+      <c r="X3" t="s">
         <v>177</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>365</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
         <v>184</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AA3" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
         <v>375</v>
       </c>
-      <c r="C4" t="s">
-        <v>27</v>
-      </c>
       <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
         <v>72</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>388</v>
       </c>
-      <c r="F4" t="s">
-        <v>524</v>
-      </c>
-      <c r="H4" t="s">
-        <v>352</v>
+      <c r="G4" t="s">
+        <v>532</v>
       </c>
       <c r="I4" t="s">
+        <v>351</v>
+      </c>
+      <c r="J4" t="s">
         <v>239</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>336</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>25</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>26</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>242</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>220</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>401</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>506</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>359</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>410</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>355</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>173</v>
       </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
         <v>178</v>
       </c>
-      <c r="X4" t="s">
+      <c r="Y4" t="s">
         <v>184</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="Z4" t="s">
         <v>518</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AA4" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
         <v>376</v>
       </c>
-      <c r="C5" t="s">
-        <v>225</v>
-      </c>
       <c r="D5" t="s">
+        <v>529</v>
+      </c>
+      <c r="E5" t="s">
         <v>493</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>337</v>
       </c>
-      <c r="F5" t="s">
-        <v>329</v>
-      </c>
-      <c r="H5" t="s">
-        <v>349</v>
+      <c r="G5" t="s">
+        <v>533</v>
       </c>
       <c r="I5" t="s">
-        <v>71</v>
-      </c>
-      <c r="K5" t="s">
+        <v>352</v>
+      </c>
+      <c r="J5" t="s">
+        <v>537</v>
+      </c>
+      <c r="L5" t="s">
         <v>86</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>30</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>243</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>221</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>402</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>507</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>360</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>356</v>
       </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
         <v>174</v>
       </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
         <v>179</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Y5" t="s">
         <v>185</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="Z5" t="s">
         <v>519</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AA5" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
         <v>377</v>
       </c>
-      <c r="C6" t="s">
-        <v>319</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" t="s">
         <v>389</v>
       </c>
-      <c r="F6" t="s">
-        <v>330</v>
+      <c r="G6" t="s">
+        <v>534</v>
       </c>
       <c r="I6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K6" t="s">
+        <v>349</v>
+      </c>
+      <c r="J6" t="s">
+        <v>71</v>
+      </c>
+      <c r="L6" t="s">
         <v>29</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>31</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>244</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>392</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>403</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>362</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>98</v>
       </c>
-      <c r="V6" t="s">
+      <c r="W6" t="s">
         <v>515</v>
       </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>180</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Y6" t="s">
         <v>186</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="Z6" t="s">
         <v>520</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AA6" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
         <v>378</v>
       </c>
-      <c r="C7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="D7" t="s">
+        <v>225</v>
+      </c>
+      <c r="F7" t="s">
         <v>367</v>
       </c>
-      <c r="F7" t="s">
-        <v>323</v>
-      </c>
-      <c r="I7" t="s">
-        <v>79</v>
-      </c>
-      <c r="K7" t="s">
+      <c r="G7" t="s">
+        <v>524</v>
+      </c>
+      <c r="J7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L7" t="s">
         <v>316</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>33</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>245</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>502</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>404</v>
       </c>
-      <c r="S7" t="s">
+      <c r="T7" t="s">
         <v>361</v>
       </c>
-      <c r="U7" t="s">
+      <c r="V7" t="s">
         <v>99</v>
       </c>
-      <c r="V7" t="s">
+      <c r="W7" t="s">
         <v>516</v>
       </c>
-      <c r="W7" t="s">
+      <c r="X7" t="s">
         <v>181</v>
       </c>
-      <c r="X7" t="s">
+      <c r="Y7" t="s">
         <v>187</v>
       </c>
-      <c r="Y7" t="s">
+      <c r="Z7" t="s">
         <v>521</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="AA7" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>348</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
         <v>379</v>
       </c>
-      <c r="C8" t="s">
-        <v>316</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="D8" t="s">
+        <v>319</v>
+      </c>
+      <c r="F8" t="s">
         <v>368</v>
       </c>
-      <c r="F8" t="s">
-        <v>324</v>
-      </c>
-      <c r="I8" t="s">
-        <v>38</v>
-      </c>
-      <c r="K8" t="s">
+      <c r="G8" t="s">
+        <v>329</v>
+      </c>
+      <c r="J8" t="s">
+        <v>79</v>
+      </c>
+      <c r="L8" t="s">
         <v>34</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>90</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>246</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>405</v>
       </c>
-      <c r="S8" t="s">
+      <c r="T8" t="s">
         <v>363</v>
       </c>
-      <c r="U8" t="s">
+      <c r="V8" t="s">
         <v>100</v>
       </c>
-      <c r="V8" t="s">
+      <c r="W8" t="s">
         <v>175</v>
       </c>
-      <c r="W8" t="s">
+      <c r="X8" t="s">
         <v>182</v>
       </c>
-      <c r="X8" t="s">
+      <c r="Y8" t="s">
         <v>188</v>
       </c>
-      <c r="Y8" t="s">
+      <c r="Z8" t="s">
         <v>522</v>
       </c>
-      <c r="Z8" t="s">
+      <c r="AA8" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>348</v>
       </c>
       <c r="B9" t="s">
         <v>380</v>
       </c>
-      <c r="C9" t="s">
-        <v>256</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" t="s">
         <v>307</v>
       </c>
-      <c r="F9" t="s">
-        <v>325</v>
-      </c>
-      <c r="I9" t="s">
-        <v>391</v>
-      </c>
-      <c r="K9" t="s">
+      <c r="G9" t="s">
+        <v>330</v>
+      </c>
+      <c r="J9" t="s">
+        <v>38</v>
+      </c>
+      <c r="L9" t="s">
         <v>35</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>91</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>247</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>406</v>
       </c>
-      <c r="S9" t="s">
+      <c r="T9" t="s">
         <v>364</v>
       </c>
-      <c r="U9" t="s">
+      <c r="V9" t="s">
         <v>210</v>
       </c>
-      <c r="X9" t="s">
+      <c r="Y9" t="s">
         <v>189</v>
       </c>
-      <c r="Z9" t="s">
+      <c r="AA9" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>334</v>
-      </c>
-      <c r="C10" t="s">
-        <v>320</v>
-      </c>
-      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" t="s">
+        <v>316</v>
+      </c>
+      <c r="F10" t="s">
         <v>353</v>
       </c>
-      <c r="F10" t="s">
-        <v>326</v>
-      </c>
-      <c r="I10" t="s">
-        <v>17</v>
-      </c>
-      <c r="K10" t="s">
+      <c r="G10" t="s">
+        <v>535</v>
+      </c>
+      <c r="J10" t="s">
+        <v>391</v>
+      </c>
+      <c r="L10" t="s">
         <v>36</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>501</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>248</v>
       </c>
-      <c r="P10" t="s">
+      <c r="Q10" t="s">
         <v>407</v>
       </c>
-      <c r="U10" t="s">
+      <c r="V10" t="s">
         <v>258</v>
       </c>
-      <c r="X10" t="s">
+      <c r="Y10" t="s">
         <v>190</v>
       </c>
-      <c r="Z10" t="s">
+      <c r="AA10" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" t="s">
-        <v>342</v>
-      </c>
-      <c r="E11" t="s">
+        <v>334</v>
+      </c>
+      <c r="D11" t="s">
+        <v>256</v>
+      </c>
+      <c r="F11" t="s">
         <v>275</v>
       </c>
-      <c r="I11" t="s">
-        <v>42</v>
-      </c>
-      <c r="K11" t="s">
+      <c r="G11" t="s">
+        <v>323</v>
+      </c>
+      <c r="J11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11" t="s">
         <v>497</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>92</v>
       </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
         <v>249</v>
       </c>
-      <c r="U11" t="s">
+      <c r="V11" t="s">
         <v>259</v>
       </c>
-      <c r="X11" t="s">
+      <c r="Y11" t="s">
         <v>260</v>
       </c>
-      <c r="Z11" t="s">
+      <c r="AA11" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>196</v>
-      </c>
-      <c r="C12" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>320</v>
+      </c>
+      <c r="F12" t="s">
         <v>264</v>
       </c>
-      <c r="I12" t="s">
-        <v>80</v>
-      </c>
-      <c r="K12" t="s">
+      <c r="G12" t="s">
+        <v>324</v>
+      </c>
+      <c r="J12" t="s">
+        <v>42</v>
+      </c>
+      <c r="L12" t="s">
         <v>39</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>41</v>
       </c>
-      <c r="N12" t="s">
+      <c r="O12" t="s">
         <v>250</v>
       </c>
-      <c r="U12" t="s">
+      <c r="V12" t="s">
         <v>101</v>
       </c>
-      <c r="X12" t="s">
+      <c r="Y12" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>51</v>
-      </c>
-      <c r="C13" t="s">
-        <v>58</v>
-      </c>
-      <c r="E13" t="s">
+        <v>196</v>
+      </c>
+      <c r="D13" t="s">
+        <v>342</v>
+      </c>
+      <c r="F13" t="s">
         <v>317</v>
       </c>
-      <c r="I13" t="s">
-        <v>81</v>
-      </c>
-      <c r="K13" t="s">
+      <c r="G13" t="s">
+        <v>325</v>
+      </c>
+      <c r="J13" t="s">
+        <v>80</v>
+      </c>
+      <c r="L13" t="s">
         <v>40</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>93</v>
       </c>
-      <c r="N13" t="s">
+      <c r="O13" t="s">
         <v>255</v>
       </c>
-      <c r="U13" t="s">
+      <c r="V13" t="s">
         <v>327</v>
       </c>
-      <c r="X13" t="s">
+      <c r="Y13" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>240</v>
-      </c>
-      <c r="C14" t="s">
-        <v>386</v>
-      </c>
-      <c r="E14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" t="s">
         <v>265</v>
       </c>
-      <c r="I14" t="s">
-        <v>82</v>
-      </c>
-      <c r="K14" t="s">
+      <c r="G14" t="s">
+        <v>326</v>
+      </c>
+      <c r="J14" t="s">
+        <v>81</v>
+      </c>
+      <c r="L14" t="s">
         <v>43</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>94</v>
       </c>
-      <c r="N14" t="s">
+      <c r="O14" t="s">
         <v>251</v>
       </c>
-      <c r="U14" t="s">
+      <c r="V14" t="s">
         <v>102</v>
       </c>
-      <c r="X14" t="s">
+      <c r="Y14" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15" t="s">
-        <v>387</v>
-      </c>
-      <c r="E15" t="s">
+        <v>240</v>
+      </c>
+      <c r="D15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" t="s">
         <v>266</v>
       </c>
-      <c r="I15" t="s">
-        <v>83</v>
-      </c>
-      <c r="M15" t="s">
+      <c r="J15" t="s">
+        <v>538</v>
+      </c>
+      <c r="N15" t="s">
         <v>95</v>
       </c>
-      <c r="N15" t="s">
+      <c r="O15" t="s">
         <v>252</v>
       </c>
-      <c r="U15" t="s">
+      <c r="V15" t="s">
         <v>103</v>
       </c>
-      <c r="X15" t="s">
+      <c r="Y15" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>397</v>
-      </c>
-      <c r="C16" t="s">
-        <v>491</v>
-      </c>
-      <c r="E16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" t="s">
+        <v>386</v>
+      </c>
+      <c r="F16" t="s">
         <v>318</v>
       </c>
-      <c r="I16" t="s">
-        <v>381</v>
-      </c>
-      <c r="N16" t="s">
+      <c r="J16" t="s">
+        <v>82</v>
+      </c>
+      <c r="O16" t="s">
         <v>253</v>
       </c>
-      <c r="U16" t="s">
+      <c r="V16" t="s">
         <v>74</v>
       </c>
-      <c r="X16" t="s">
+      <c r="Y16" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>488</v>
-      </c>
-      <c r="C17" t="s">
-        <v>59</v>
-      </c>
-      <c r="E17" t="s">
+        <v>397</v>
+      </c>
+      <c r="D17" t="s">
+        <v>387</v>
+      </c>
+      <c r="F17" t="s">
         <v>88</v>
       </c>
-      <c r="I17" t="s">
-        <v>44</v>
-      </c>
-      <c r="U17" t="s">
+      <c r="J17" t="s">
+        <v>83</v>
+      </c>
+      <c r="V17" t="s">
         <v>104</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>543</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>489</v>
-      </c>
-      <c r="C18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E18" t="s">
+        <v>488</v>
+      </c>
+      <c r="D18" t="s">
+        <v>491</v>
+      </c>
+      <c r="F18" t="s">
         <v>89</v>
       </c>
-      <c r="I18" t="s">
-        <v>393</v>
-      </c>
-      <c r="U18" t="s">
+      <c r="J18" t="s">
+        <v>381</v>
+      </c>
+      <c r="V18" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>358</v>
-      </c>
-      <c r="C19" t="s">
-        <v>257</v>
-      </c>
-      <c r="E19" t="s">
+        <v>489</v>
+      </c>
+      <c r="D19" t="s">
+        <v>59</v>
+      </c>
+      <c r="F19" t="s">
         <v>297</v>
       </c>
-      <c r="I19" t="s">
-        <v>84</v>
-      </c>
-      <c r="U19" t="s">
+      <c r="J19" t="s">
+        <v>44</v>
+      </c>
+      <c r="V19" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>398</v>
-      </c>
-      <c r="C20" t="s">
-        <v>61</v>
-      </c>
-      <c r="E20" t="s">
+        <v>358</v>
+      </c>
+      <c r="D20" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20" t="s">
         <v>298</v>
       </c>
-      <c r="I20" t="s">
-        <v>495</v>
-      </c>
-      <c r="U20" t="s">
+      <c r="J20" t="s">
+        <v>393</v>
+      </c>
+      <c r="V20" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21" t="s">
-        <v>322</v>
-      </c>
-      <c r="E21" t="s">
+        <v>398</v>
+      </c>
+      <c r="D21" t="s">
+        <v>257</v>
+      </c>
+      <c r="F21" t="s">
         <v>299</v>
       </c>
-      <c r="I21" t="s">
-        <v>45</v>
-      </c>
-      <c r="U21" t="s">
+      <c r="J21" t="s">
+        <v>84</v>
+      </c>
+      <c r="V21" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" t="s">
-        <v>62</v>
-      </c>
-      <c r="E22" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" t="s">
+        <v>61</v>
+      </c>
+      <c r="F22" t="s">
         <v>300</v>
       </c>
-      <c r="I22" t="s">
-        <v>46</v>
-      </c>
-      <c r="U22" t="s">
+      <c r="J22" t="s">
+        <v>495</v>
+      </c>
+      <c r="V22" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23" t="s">
-        <v>226</v>
-      </c>
-      <c r="E23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" t="s">
+        <v>322</v>
+      </c>
+      <c r="F23" t="s">
         <v>291</v>
       </c>
-      <c r="U23" t="s">
+      <c r="J23" t="s">
+        <v>45</v>
+      </c>
+      <c r="V23" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>56</v>
-      </c>
-      <c r="C24" t="s">
-        <v>227</v>
-      </c>
-      <c r="E24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" t="s">
+        <v>62</v>
+      </c>
+      <c r="F24" t="s">
         <v>280</v>
       </c>
-      <c r="U24" t="s">
+      <c r="J24" t="s">
+        <v>46</v>
+      </c>
+      <c r="V24" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>490</v>
-      </c>
-      <c r="C25" t="s">
-        <v>492</v>
-      </c>
-      <c r="E25" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" t="s">
+        <v>530</v>
+      </c>
+      <c r="F25" t="s">
         <v>75</v>
       </c>
-      <c r="U25" t="s">
+      <c r="V25" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
+        <v>490</v>
+      </c>
+      <c r="D26" t="s">
+        <v>226</v>
+      </c>
+      <c r="F26" t="s">
+        <v>283</v>
+      </c>
+      <c r="V26" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
         <v>228</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D27" t="s">
+        <v>227</v>
+      </c>
+      <c r="F27" t="s">
+        <v>267</v>
+      </c>
+      <c r="V27" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="D28" t="s">
+        <v>492</v>
+      </c>
+      <c r="F28" t="s">
+        <v>284</v>
+      </c>
+      <c r="V28" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="D29" t="s">
         <v>63</v>
       </c>
-      <c r="E26" t="s">
-        <v>283</v>
-      </c>
-      <c r="U26" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="C27" t="s">
+      <c r="F29" t="s">
+        <v>285</v>
+      </c>
+      <c r="V29" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="D30" t="s">
         <v>64</v>
       </c>
-      <c r="E27" t="s">
-        <v>267</v>
-      </c>
-      <c r="U27" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="C28" t="s">
+      <c r="F30" t="s">
+        <v>217</v>
+      </c>
+      <c r="V30" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="D31" t="s">
         <v>65</v>
       </c>
-      <c r="E28" t="s">
-        <v>284</v>
-      </c>
-      <c r="U28" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="C29" t="s">
+      <c r="F31" t="s">
+        <v>276</v>
+      </c>
+      <c r="V31" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="D32" t="s">
         <v>66</v>
       </c>
-      <c r="E29" t="s">
-        <v>285</v>
-      </c>
-      <c r="U29" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="C30" t="s">
+      <c r="F32" t="s">
+        <v>286</v>
+      </c>
+      <c r="V32" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="D33" t="s">
         <v>67</v>
       </c>
-      <c r="E30" t="s">
-        <v>217</v>
-      </c>
-      <c r="U30" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="C31" t="s">
+      <c r="F33" t="s">
+        <v>261</v>
+      </c>
+      <c r="V33" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="D34" t="s">
         <v>68</v>
       </c>
-      <c r="E31" t="s">
-        <v>276</v>
-      </c>
-      <c r="U31" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="C32" t="s">
+      <c r="F34" t="s">
+        <v>331</v>
+      </c>
+      <c r="V34" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="D35" t="s">
         <v>69</v>
       </c>
-      <c r="E32" t="s">
-        <v>286</v>
-      </c>
-      <c r="U32" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="C33" t="s">
+      <c r="F35" t="s">
+        <v>308</v>
+      </c>
+      <c r="V35" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="D36" t="s">
         <v>70</v>
       </c>
-      <c r="E33" t="s">
-        <v>261</v>
-      </c>
-      <c r="U33" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="E34" t="s">
-        <v>331</v>
-      </c>
-      <c r="U34" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="E35" t="s">
-        <v>308</v>
-      </c>
-      <c r="U35" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="E36" t="s">
+      <c r="F36" t="s">
         <v>262</v>
       </c>
-      <c r="U36" t="s">
+      <c r="V36" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="37">
-      <c r="E37" t="s">
+      <c r="F37" t="s">
         <v>309</v>
       </c>
-      <c r="U37" t="s">
+      <c r="V37" t="s">
         <v>508</v>
       </c>
     </row>
     <row r="38">
-      <c r="E38" t="s">
+      <c r="F38" t="s">
         <v>268</v>
       </c>
-      <c r="U38" t="s">
+      <c r="V38" t="s">
         <v>394</v>
       </c>
     </row>
     <row r="39">
-      <c r="E39" t="s">
+      <c r="F39" t="s">
         <v>77</v>
       </c>
-      <c r="U39" t="s">
+      <c r="V39" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="40">
-      <c r="E40" t="s">
+      <c r="F40" t="s">
         <v>213</v>
       </c>
-      <c r="U40" t="s">
+      <c r="V40" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="41">
-      <c r="E41" t="s">
+      <c r="F41" t="s">
         <v>290</v>
       </c>
-      <c r="U41" t="s">
+      <c r="V41" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="42">
-      <c r="E42" t="s">
+      <c r="F42" t="s">
         <v>301</v>
       </c>
-      <c r="U42" t="s">
+      <c r="V42" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="43">
-      <c r="E43" t="s">
+      <c r="F43" t="s">
         <v>302</v>
       </c>
-      <c r="U43" t="s">
+      <c r="V43" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="44">
-      <c r="E44" t="s">
+      <c r="F44" t="s">
         <v>344</v>
       </c>
-      <c r="U44" t="s">
+      <c r="V44" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="45">
-      <c r="E45" t="s">
+      <c r="F45" t="s">
         <v>343</v>
       </c>
-      <c r="U45" t="s">
+      <c r="V45" t="s">
         <v>509</v>
       </c>
     </row>
     <row r="46">
-      <c r="E46" t="s">
+      <c r="F46" t="s">
         <v>212</v>
       </c>
-      <c r="U46" t="s">
+      <c r="V46" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="47">
-      <c r="E47" t="s">
+      <c r="F47" t="s">
         <v>321</v>
       </c>
-      <c r="U47" t="s">
+      <c r="V47" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="48">
-      <c r="E48" t="s">
+      <c r="F48" t="s">
         <v>340</v>
       </c>
-      <c r="U48" t="s">
+      <c r="V48" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="49">
-      <c r="E49" t="s">
+      <c r="F49" t="s">
         <v>369</v>
       </c>
-      <c r="U49" t="s">
+      <c r="V49" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="50">
-      <c r="E50" t="s">
+      <c r="F50" t="s">
         <v>303</v>
       </c>
-      <c r="U50" t="s">
+      <c r="V50" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="51">
-      <c r="E51" t="s">
+      <c r="F51" t="s">
         <v>357</v>
       </c>
-      <c r="U51" t="s">
+      <c r="V51" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="F52" t="s">
+        <v>332</v>
+      </c>
+      <c r="V52" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="52">
-      <c r="E52" t="s">
-        <v>332</v>
-      </c>
-      <c r="U52" t="s">
+    <row r="53">
+      <c r="F53" t="s">
+        <v>269</v>
+      </c>
+      <c r="V53" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="53">
-      <c r="E53" t="s">
-        <v>269</v>
-      </c>
-      <c r="U53" t="s">
+    <row r="54">
+      <c r="F54" t="s">
+        <v>293</v>
+      </c>
+      <c r="V54" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="F55" t="s">
+        <v>294</v>
+      </c>
+      <c r="V55" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="54">
-      <c r="E54" t="s">
-        <v>293</v>
-      </c>
-      <c r="U54" t="s">
+    <row r="56">
+      <c r="F56" t="s">
+        <v>295</v>
+      </c>
+      <c r="V56" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="55">
-      <c r="E55" t="s">
-        <v>294</v>
-      </c>
-      <c r="U55" t="s">
+    <row r="57">
+      <c r="F57" t="s">
+        <v>304</v>
+      </c>
+      <c r="V57" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="56">
-      <c r="E56" t="s">
-        <v>295</v>
-      </c>
-      <c r="U56" t="s">
+    <row r="58">
+      <c r="F58" t="s">
+        <v>313</v>
+      </c>
+      <c r="V58" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="57">
-      <c r="E57" t="s">
-        <v>304</v>
-      </c>
-      <c r="U57" t="s">
+    <row r="59">
+      <c r="F59" t="s">
+        <v>338</v>
+      </c>
+      <c r="V59" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="58">
-      <c r="E58" t="s">
-        <v>313</v>
-      </c>
-      <c r="U58" t="s">
+    <row r="60">
+      <c r="F60" t="s">
+        <v>310</v>
+      </c>
+      <c r="V60" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="59">
-      <c r="E59" t="s">
-        <v>338</v>
-      </c>
-      <c r="U59" t="s">
+    <row r="61">
+      <c r="F61" t="s">
+        <v>311</v>
+      </c>
+      <c r="V61" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="60">
-      <c r="E60" t="s">
-        <v>310</v>
-      </c>
-      <c r="U60" t="s">
+    <row r="62">
+      <c r="F62" t="s">
+        <v>370</v>
+      </c>
+      <c r="V62" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="61">
-      <c r="E61" t="s">
-        <v>311</v>
-      </c>
-      <c r="U61" t="s">
+    <row r="63">
+      <c r="F63" t="s">
+        <v>371</v>
+      </c>
+      <c r="V63" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="62">
-      <c r="E62" t="s">
-        <v>370</v>
-      </c>
-      <c r="U62" t="s">
+    <row r="64">
+      <c r="F64" t="s">
+        <v>346</v>
+      </c>
+      <c r="V64" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="63">
-      <c r="E63" t="s">
-        <v>371</v>
-      </c>
-      <c r="U63" t="s">
+    <row r="65">
+      <c r="F65" t="s">
+        <v>314</v>
+      </c>
+      <c r="V65" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="64">
-      <c r="E64" t="s">
-        <v>346</v>
-      </c>
-      <c r="U64" t="s">
+    <row r="66">
+      <c r="F66" t="s">
+        <v>270</v>
+      </c>
+      <c r="V66" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="65">
-      <c r="E65" t="s">
-        <v>314</v>
-      </c>
-      <c r="U65" t="s">
+    <row r="67">
+      <c r="F67" t="s">
+        <v>354</v>
+      </c>
+      <c r="V67" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="66">
-      <c r="E66" t="s">
-        <v>270</v>
-      </c>
-      <c r="U66" t="s">
+    <row r="68">
+      <c r="F68" t="s">
+        <v>315</v>
+      </c>
+      <c r="V68" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="67">
-      <c r="E67" t="s">
-        <v>354</v>
-      </c>
-      <c r="U67" t="s">
+    <row r="69">
+      <c r="F69" t="s">
+        <v>411</v>
+      </c>
+      <c r="V69" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="68">
-      <c r="E68" t="s">
-        <v>315</v>
-      </c>
-      <c r="U68" t="s">
+    <row r="70">
+      <c r="F70" t="s">
+        <v>305</v>
+      </c>
+      <c r="V70" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="69">
-      <c r="E69" t="s">
-        <v>411</v>
-      </c>
-      <c r="U69" t="s">
+    <row r="71">
+      <c r="F71" t="s">
+        <v>412</v>
+      </c>
+      <c r="V71" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="70">
-      <c r="E70" t="s">
-        <v>305</v>
-      </c>
-      <c r="U70" t="s">
+    <row r="72">
+      <c r="F72" t="s">
+        <v>263</v>
+      </c>
+      <c r="V72" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="F73" t="s">
+        <v>345</v>
+      </c>
+      <c r="V73" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="71">
-      <c r="E71" t="s">
-        <v>412</v>
-      </c>
-      <c r="U71" t="s">
+    <row r="74">
+      <c r="F74" t="s">
+        <v>281</v>
+      </c>
+      <c r="V74" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="72">
-      <c r="E72" t="s">
-        <v>263</v>
-      </c>
-      <c r="U72" t="s">
+    <row r="75">
+      <c r="F75" t="s">
+        <v>287</v>
+      </c>
+      <c r="V75" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="73">
-      <c r="E73" t="s">
-        <v>345</v>
-      </c>
-      <c r="U73" t="s">
+    <row r="76">
+      <c r="F76" t="s">
+        <v>292</v>
+      </c>
+      <c r="V76" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="74">
-      <c r="E74" t="s">
-        <v>281</v>
-      </c>
-      <c r="U74" t="s">
+    <row r="77">
+      <c r="F77" t="s">
+        <v>494</v>
+      </c>
+      <c r="V77" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="75">
-      <c r="E75" t="s">
-        <v>287</v>
-      </c>
-      <c r="U75" t="s">
+    <row r="78">
+      <c r="F78" t="s">
+        <v>333</v>
+      </c>
+      <c r="V78" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="76">
-      <c r="E76" t="s">
-        <v>292</v>
-      </c>
-      <c r="U76" t="s">
+    <row r="79">
+      <c r="F79" t="s">
+        <v>271</v>
+      </c>
+      <c r="V79" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="77">
-      <c r="E77" t="s">
-        <v>494</v>
-      </c>
-      <c r="U77" t="s">
+    <row r="80">
+      <c r="F80" t="s">
+        <v>282</v>
+      </c>
+      <c r="V80" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="F81" t="s">
+        <v>288</v>
+      </c>
+      <c r="V81" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="78">
-      <c r="E78" t="s">
-        <v>333</v>
-      </c>
-      <c r="U78" t="s">
+    <row r="82">
+      <c r="F82" t="s">
+        <v>277</v>
+      </c>
+      <c r="V82" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="79">
-      <c r="E79" t="s">
-        <v>271</v>
-      </c>
-      <c r="U79" t="s">
+    <row r="83">
+      <c r="F83" t="s">
+        <v>272</v>
+      </c>
+      <c r="V83" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="80">
-      <c r="E80" t="s">
-        <v>282</v>
-      </c>
-      <c r="U80" t="s">
+    <row r="84">
+      <c r="F84" t="s">
+        <v>289</v>
+      </c>
+      <c r="V84" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="81">
-      <c r="E81" t="s">
-        <v>288</v>
-      </c>
-      <c r="U81" t="s">
+    <row r="85">
+      <c r="F85" t="s">
+        <v>273</v>
+      </c>
+      <c r="V85" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="82">
-      <c r="E82" t="s">
-        <v>277</v>
-      </c>
-      <c r="U82" t="s">
+    <row r="86">
+      <c r="F86" t="s">
+        <v>274</v>
+      </c>
+      <c r="V86" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="83">
-      <c r="E83" t="s">
-        <v>272</v>
-      </c>
-      <c r="U83" t="s">
+    <row r="87">
+      <c r="F87" t="s">
+        <v>306</v>
+      </c>
+      <c r="V87" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="84">
-      <c r="E84" t="s">
-        <v>289</v>
-      </c>
-      <c r="U84" t="s">
+    <row r="88">
+      <c r="F88" t="s">
+        <v>312</v>
+      </c>
+      <c r="V88" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="85">
-      <c r="E85" t="s">
-        <v>273</v>
-      </c>
-      <c r="U85" t="s">
+    <row r="89">
+      <c r="F89" t="s">
+        <v>296</v>
+      </c>
+      <c r="V89" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="86">
-      <c r="E86" t="s">
-        <v>274</v>
-      </c>
-      <c r="U86" t="s">
+    <row r="90">
+      <c r="F90" t="s">
+        <v>341</v>
+      </c>
+      <c r="V90" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="87">
-      <c r="E87" t="s">
-        <v>306</v>
-      </c>
-      <c r="U87" t="s">
+    <row r="91">
+      <c r="F91" t="s">
+        <v>278</v>
+      </c>
+      <c r="V91" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="88">
-      <c r="E88" t="s">
-        <v>312</v>
-      </c>
-      <c r="U88" t="s">
+    <row r="92">
+      <c r="F92" t="s">
+        <v>279</v>
+      </c>
+      <c r="V92" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="89">
-      <c r="E89" t="s">
-        <v>296</v>
-      </c>
-      <c r="U89" t="s">
+    <row r="93">
+      <c r="V93" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="90">
-      <c r="E90" t="s">
-        <v>341</v>
-      </c>
-      <c r="U90" t="s">
+    <row r="94">
+      <c r="V94" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="91">
-      <c r="E91" t="s">
-        <v>278</v>
-      </c>
-      <c r="U91" t="s">
+    <row r="95">
+      <c r="V95" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="92">
-      <c r="E92" t="s">
-        <v>279</v>
-      </c>
-      <c r="U92" t="s">
+    <row r="96">
+      <c r="V96" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="93">
-      <c r="U93" t="s">
+    <row r="97">
+      <c r="V97" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="94">
-      <c r="U94" t="s">
+    <row r="98">
+      <c r="V98" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="95">
-      <c r="U95" t="s">
+    <row r="99">
+      <c r="V99" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="96">
-      <c r="U96" t="s">
+    <row r="100">
+      <c r="V100" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="97">
-      <c r="U97" t="s">
+    <row r="101">
+      <c r="V101" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="98">
-      <c r="U98" t="s">
+    <row r="102">
+      <c r="V102" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="99">
-      <c r="U99" t="s">
+    <row r="103">
+      <c r="V103" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="100">
-      <c r="U100" t="s">
+    <row r="104">
+      <c r="V104" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="101">
-      <c r="U101" t="s">
+    <row r="105">
+      <c r="V105" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="102">
-      <c r="U102" t="s">
+    <row r="106">
+      <c r="V106" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="103">
-      <c r="U103" t="s">
+    <row r="107">
+      <c r="V107" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="104">
-      <c r="U104" t="s">
+    <row r="108">
+      <c r="V108" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="105">
-      <c r="U105" t="s">
+    <row r="109">
+      <c r="V109" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="106">
-      <c r="U106" t="s">
+    <row r="110">
+      <c r="V110" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="107">
-      <c r="U107" t="s">
+    <row r="111">
+      <c r="V111" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="108">
-      <c r="U108" t="s">
+    <row r="112">
+      <c r="V112" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="109">
-      <c r="U109" t="s">
+    <row r="113">
+      <c r="V113" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="110">
-      <c r="U110" t="s">
+    <row r="114">
+      <c r="V114" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="111">
-      <c r="U111" t="s">
+    <row r="115">
+      <c r="V115" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="112">
-      <c r="U112" t="s">
+    <row r="116">
+      <c r="V116" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="113">
-      <c r="U113" t="s">
+    <row r="117">
+      <c r="V117" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="114">
-      <c r="U114" t="s">
+    <row r="118">
+      <c r="V118" t="s">
         <v>170</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- block the display of crypted data variables
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/demo1/artifact/script/InjestData.xlsx
+++ b/demo1/artifact/script/InjestData.xlsx
@@ -20,37 +20,39 @@
   </sheets>
   <definedNames>
     <definedName name="aws.s3">'#system'!$B$2:$B$9</definedName>
-    <definedName name="base">'#system'!$D$2:$D$38</definedName>
-    <definedName name="csv">'#system'!$E$2:$E$5</definedName>
+    <definedName name="base">'#system'!$E$2:$E$38</definedName>
+    <definedName name="csv">'#system'!$F$2:$F$6</definedName>
     <definedName name="date">'#system'!$C$2:$C$14</definedName>
     <definedName name="db">'#system'!$D$2:$D$5</definedName>
-    <definedName name="desktop">'#system'!$F$2:$F$92</definedName>
-    <definedName name="excel">'#system'!$G$2:$G$14</definedName>
-    <definedName name="external">'#system'!$H$2:$H$3</definedName>
-    <definedName name="image">'#system'!$I$2:$I$6</definedName>
-    <definedName name="io">'#system'!$J$2:$J$25</definedName>
-    <definedName name="jms">'#system'!$K$2:$K$4</definedName>
-    <definedName name="json">'#system'!$L$2:$L$14</definedName>
-    <definedName name="mail">'#system'!$M$2:$M$2</definedName>
+    <definedName name="desktop">'#system'!$G$2:$G$94</definedName>
+    <definedName name="excel">'#system'!$H$2:$H$14</definedName>
+    <definedName name="external">'#system'!$I$2:$I$4</definedName>
+    <definedName name="image">'#system'!$J$2:$J$6</definedName>
+    <definedName name="io">'#system'!$K$2:$K$28</definedName>
+    <definedName name="jms">'#system'!$L$2:$L$4</definedName>
+    <definedName name="json">'#system'!$M$2:$M$16</definedName>
+    <definedName name="mail">'#system'!$O$2:$O$2</definedName>
     <definedName name="math">'#system'!$K$2:$K$13</definedName>
     <definedName name="mq">'#system'!$J$2:$J$3</definedName>
     <definedName name="nextgen">'#system'!$K$2:$K$28</definedName>
-    <definedName name="number">'#system'!$N$2:$N$15</definedName>
-    <definedName name="pdf">'#system'!$O$2:$O$16</definedName>
-    <definedName name="rdbms">'#system'!$P$2:$P$7</definedName>
-    <definedName name="redis">'#system'!$Q$2:$Q$10</definedName>
-    <definedName name="ssh">'#system'!$T$2:$T$9</definedName>
-    <definedName name="step">'#system'!$U$2:$U$4</definedName>
-    <definedName name="target">'#system'!$A$2:$A$27</definedName>
-    <definedName name="web">'#system'!$V$2:$V$119</definedName>
-    <definedName name="webalert">'#system'!$W$2:$W$8</definedName>
-    <definedName name="webcookie">'#system'!$X$2:$X$8</definedName>
-    <definedName name="ws">'#system'!$Y$2:$Y$17</definedName>
-    <definedName name="xml">'#system'!$AA$2:$AA$11</definedName>
-    <definedName name="sms">'#system'!$R$2:$R$2</definedName>
-    <definedName name="sound">'#system'!$S$2:$S$5</definedName>
-    <definedName name="ws.async">'#system'!$Z$2:$Z$8</definedName>
+    <definedName name="number">'#system'!$P$2:$P$16</definedName>
+    <definedName name="pdf">'#system'!$Q$2:$Q$16</definedName>
+    <definedName name="rdbms">'#system'!$R$2:$R$7</definedName>
+    <definedName name="redis">'#system'!$S$2:$S$10</definedName>
+    <definedName name="ssh">'#system'!$V$2:$V$9</definedName>
+    <definedName name="step">'#system'!$W$2:$W$4</definedName>
+    <definedName name="target">'#system'!$A$2:$A$29</definedName>
+    <definedName name="web">'#system'!$X$2:$X$125</definedName>
+    <definedName name="webalert">'#system'!$Y$2:$Y$8</definedName>
+    <definedName name="webcookie">'#system'!$Z$2:$Z$8</definedName>
+    <definedName name="ws">'#system'!$AA$2:$AA$17</definedName>
+    <definedName name="xml">'#system'!$AC$2:$AC$21</definedName>
+    <definedName name="sms">'#system'!$T$2:$T$2</definedName>
+    <definedName name="sound">'#system'!$U$2:$U$5</definedName>
+    <definedName name="ws.async">'#system'!$AB$2:$AB$8</definedName>
     <definedName name="aws.ses">'#system'!$C$2:$C$3</definedName>
+    <definedName name="aws.sqs">'#system'!$D$2:$D$5</definedName>
+    <definedName name="macro">'#system'!$N$2:$N$4</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
@@ -70,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3470" uniqueCount="548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3988" uniqueCount="586">
   <si>
     <t>description</t>
   </si>
@@ -1715,6 +1717,120 @@
   </si>
   <si>
     <t>searchAndReplace(file,config,saveAs)</t>
+  </si>
+  <si>
+    <t>aws.sqs</t>
+  </si>
+  <si>
+    <t>macro</t>
+  </si>
+  <si>
+    <t>deleteMessage(profile,queue,receiptHandle)</t>
+  </si>
+  <si>
+    <t>receiveMessage(profile,queue,var)</t>
+  </si>
+  <si>
+    <t>receiveMessages(profile,queue,var)</t>
+  </si>
+  <si>
+    <t>sendMessage(profile,queue,message,var)</t>
+  </si>
+  <si>
+    <t>toExcel(csvFile,excel,worksheet,startCell)</t>
+  </si>
+  <si>
+    <t>clickElementOffset(name,xOffset,yOffset)</t>
+  </si>
+  <si>
+    <t>saveTextByLocator(var,locator)</t>
+  </si>
+  <si>
+    <t>runProgram(programPathAndParams)</t>
+  </si>
+  <si>
+    <t>runProgramNoWait(programPathAndParams)</t>
+  </si>
+  <si>
+    <t>copyFilesByRegex(sourceDir,regex,target)</t>
+  </si>
+  <si>
+    <t>deleteFilesByRegex(sourceDir,regex)</t>
+  </si>
+  <si>
+    <t>moveFilesByRegex(sourceDir,regex,target)</t>
+  </si>
+  <si>
+    <t>beautify(json,var)</t>
+  </si>
+  <si>
+    <t>minify(json,var)</t>
+  </si>
+  <si>
+    <t>description()</t>
+  </si>
+  <si>
+    <t>expects(var,default)</t>
+  </si>
+  <si>
+    <t>produces(var,value)</t>
+  </si>
+  <si>
+    <t>roundTo(var,closestDigit)</t>
+  </si>
+  <si>
+    <t>whole(var)</t>
+  </si>
+  <si>
+    <t>assertElementsPresent(prefix)</t>
+  </si>
+  <si>
+    <t>assertIENativeMode()</t>
+  </si>
+  <si>
+    <t>clickOffset(locator,x,y)</t>
+  </si>
+  <si>
+    <t>dragTo(fromLocator,xOffset,yOffset)</t>
+  </si>
+  <si>
+    <t>rightClick(locator)</t>
+  </si>
+  <si>
+    <t>saveAttributeList(var,locator,attrName)</t>
+  </si>
+  <si>
+    <t>saveValues(var,locator)</t>
+  </si>
+  <si>
+    <t>append(xml,xpath,content,var)</t>
+  </si>
+  <si>
+    <t>beautify(xml,var)</t>
+  </si>
+  <si>
+    <t>clear(xml,xpath,var)</t>
+  </si>
+  <si>
+    <t>delete(xml,xpath,var)</t>
+  </si>
+  <si>
+    <t>insertAfter(xml,xpath,content,var)</t>
+  </si>
+  <si>
+    <t>insertBefore(xml,xpath,content,var)</t>
+  </si>
+  <si>
+    <t>minify(xml,var)</t>
+  </si>
+  <si>
+    <t>prepend(xml,xpath,content,var)</t>
+  </si>
+  <si>
+    <t>replace(xml,xpath,content,var)</t>
+  </si>
+  <si>
+    <t>replaceIn(xml,xpath,content,var)</t>
   </si>
 </sst>
 </file>
@@ -1722,7 +1838,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="107" x14ac:knownFonts="1">
+  <fonts count="123" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2405,8 +2521,109 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="823C3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="167">
+  <fills count="194">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3349,8 +3566,161 @@
         <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="174">
+  <borders count="202">
     <border>
       <left/>
       <right/>
@@ -5117,6 +5487,288 @@
         <color rgb="C3C3C3"/>
       </bottom>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
@@ -5124,7 +5776,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="138">
+  <cellXfs count="154">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="2" fontId="7" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -5515,52 +6167,100 @@
     <xf applyFont="true" borderId="0" fillId="0" fontId="90" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="91" fillId="142" borderId="153" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="153" fillId="142" fontId="91" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="92" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="92" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="93" fillId="145" borderId="157" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="157" fillId="145" fontId="93" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="94" fillId="148" borderId="161" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="161" fillId="148" fontId="94" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="95" fillId="151" borderId="161" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="161" fillId="151" fontId="95" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="96" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="96" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="97" fillId="154" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="154" fontId="97" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="98" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="98" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="99" fillId="157" borderId="165" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="165" fillId="157" fontId="99" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="100" fillId="160" borderId="169" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="169" fillId="160" fontId="100" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="101" fillId="163" borderId="173" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="173" fillId="163" fontId="101" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="102" fillId="163" borderId="173" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="173" fillId="163" fontId="102" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="103" fillId="151" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="151" fontId="103" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="104" fillId="166" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="166" fontId="104" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="105" fillId="151" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="151" fontId="105" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="106" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="106" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="107" fillId="169" borderId="181" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="108" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="109" fillId="172" borderId="185" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="110" fillId="175" borderId="189" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="111" fillId="178" borderId="189" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="112" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="113" fillId="181" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="114" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="115" fillId="184" borderId="193" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="116" fillId="187" borderId="197" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="117" fillId="190" borderId="201" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="118" fillId="190" borderId="201" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="119" fillId="178" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="120" fillId="193" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="121" fillId="178" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="122" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -5945,7 +6645,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB119"/>
+  <dimension ref="A1:AD125"/>
   <sheetViews>
     <sheetView tabSelected="false" workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125">
       <selection activeCell="A19" sqref="A19"/>
@@ -5967,75 +6667,81 @@
         <v>525</v>
       </c>
       <c r="D1" t="s">
+        <v>548</v>
+      </c>
+      <c r="E1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>50</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>22</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>23</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>348</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>334</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>24</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
+        <v>549</v>
+      </c>
+      <c r="O1" t="s">
         <v>196</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>51</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>240</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>52</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>397</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>488</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>489</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>358</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>398</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>53</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>54</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>55</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>56</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>490</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>228</v>
       </c>
     </row>
@@ -6050,76 +6756,82 @@
         <v>526</v>
       </c>
       <c r="D2" t="s">
+        <v>550</v>
+      </c>
+      <c r="E2" t="s">
         <v>57</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>71</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>73</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>531</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>78</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>536</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>316</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>385</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>496</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
+        <v>564</v>
+      </c>
+      <c r="O2" t="s">
         <v>498</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>499</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
         <v>254</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>218</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="S2" t="s">
         <v>399</v>
       </c>
-      <c r="R2" t="s">
+      <c r="T2" t="s">
         <v>503</v>
       </c>
-      <c r="S2" t="s">
+      <c r="U2" t="s">
         <v>504</v>
       </c>
-      <c r="T2" t="s">
+      <c r="V2" t="s">
         <v>382</v>
       </c>
-      <c r="U2" t="s">
+      <c r="W2" t="s">
         <v>408</v>
       </c>
-      <c r="V2" t="s">
+      <c r="X2" t="s">
         <v>96</v>
       </c>
-      <c r="W2" t="s">
+      <c r="Y2" t="s">
         <v>171</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Z2" t="s">
         <v>176</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="AA2" t="s">
         <v>183</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AB2" t="s">
         <v>517</v>
       </c>
-      <c r="AA2" t="s">
-        <v>229</v>
+      <c r="AC2" t="s">
+        <v>576</v>
       </c>
     </row>
     <row r="3">
@@ -6133,1507 +6845,1618 @@
         <v>527</v>
       </c>
       <c r="D3" t="s">
+        <v>551</v>
+      </c>
+      <c r="E3" t="s">
         <v>528</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>366</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>87</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>48</v>
       </c>
-      <c r="H3" t="s">
-        <v>28</v>
-      </c>
       <c r="I3" t="s">
+        <v>557</v>
+      </c>
+      <c r="J3" t="s">
         <v>350</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>342</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>335</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>85</v>
       </c>
       <c r="N3" t="s">
+        <v>565</v>
+      </c>
+      <c r="P3" t="s">
         <v>500</v>
       </c>
-      <c r="O3" t="s">
+      <c r="Q3" t="s">
         <v>241</v>
       </c>
-      <c r="P3" t="s">
+      <c r="R3" t="s">
         <v>219</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="S3" t="s">
         <v>400</v>
       </c>
-      <c r="S3" t="s">
+      <c r="U3" t="s">
         <v>505</v>
       </c>
-      <c r="T3" t="s">
+      <c r="V3" t="s">
         <v>383</v>
       </c>
-      <c r="U3" t="s">
+      <c r="W3" t="s">
         <v>409</v>
       </c>
-      <c r="V3" t="s">
+      <c r="X3" t="s">
         <v>97</v>
       </c>
-      <c r="W3" t="s">
+      <c r="Y3" t="s">
         <v>172</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Z3" t="s">
         <v>177</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="AA3" t="s">
         <v>365</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AB3" t="s">
         <v>184</v>
       </c>
-      <c r="AA3" t="s">
-        <v>230</v>
+      <c r="AC3" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>548</v>
       </c>
       <c r="B4" t="s">
         <v>375</v>
       </c>
       <c r="D4" t="s">
+        <v>552</v>
+      </c>
+      <c r="E4" t="s">
         <v>15</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>72</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>388</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>532</v>
       </c>
       <c r="I4" t="s">
+        <v>558</v>
+      </c>
+      <c r="J4" t="s">
         <v>351</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>239</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>336</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>25</v>
       </c>
       <c r="N4" t="s">
+        <v>566</v>
+      </c>
+      <c r="P4" t="s">
         <v>26</v>
       </c>
-      <c r="O4" t="s">
+      <c r="Q4" t="s">
         <v>242</v>
       </c>
-      <c r="P4" t="s">
+      <c r="R4" t="s">
         <v>220</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="S4" t="s">
         <v>401</v>
       </c>
-      <c r="S4" t="s">
+      <c r="U4" t="s">
         <v>506</v>
       </c>
-      <c r="T4" t="s">
+      <c r="V4" t="s">
         <v>359</v>
       </c>
-      <c r="U4" t="s">
+      <c r="W4" t="s">
         <v>410</v>
       </c>
-      <c r="V4" t="s">
+      <c r="X4" t="s">
         <v>355</v>
       </c>
-      <c r="W4" t="s">
+      <c r="Y4" t="s">
         <v>173</v>
       </c>
-      <c r="X4" t="s">
+      <c r="Z4" t="s">
         <v>178</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="AA4" t="s">
         <v>184</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AB4" t="s">
         <v>518</v>
       </c>
-      <c r="AA4" t="s">
-        <v>231</v>
+      <c r="AC4" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
         <v>376</v>
       </c>
       <c r="D5" t="s">
+        <v>553</v>
+      </c>
+      <c r="E5" t="s">
         <v>529</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>493</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>337</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>533</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>352</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>537</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>86</v>
       </c>
-      <c r="N5" t="s">
+      <c r="P5" t="s">
         <v>30</v>
       </c>
-      <c r="O5" t="s">
+      <c r="Q5" t="s">
         <v>243</v>
       </c>
-      <c r="P5" t="s">
+      <c r="R5" t="s">
         <v>221</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="S5" t="s">
         <v>402</v>
       </c>
-      <c r="S5" t="s">
+      <c r="U5" t="s">
         <v>507</v>
       </c>
-      <c r="T5" t="s">
+      <c r="V5" t="s">
         <v>360</v>
       </c>
-      <c r="V5" t="s">
+      <c r="X5" t="s">
         <v>356</v>
       </c>
-      <c r="W5" t="s">
+      <c r="Y5" t="s">
         <v>174</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Z5" t="s">
         <v>179</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="AA5" t="s">
         <v>185</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AB5" t="s">
         <v>519</v>
       </c>
-      <c r="AA5" t="s">
-        <v>232</v>
+      <c r="AC5" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
         <v>377</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>27</v>
       </c>
       <c r="F6" t="s">
+        <v>554</v>
+      </c>
+      <c r="G6" t="s">
         <v>389</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>534</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>349</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>71</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>29</v>
       </c>
-      <c r="N6" t="s">
+      <c r="P6" t="s">
         <v>31</v>
       </c>
-      <c r="O6" t="s">
+      <c r="Q6" t="s">
         <v>244</v>
       </c>
-      <c r="P6" t="s">
+      <c r="R6" t="s">
         <v>392</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="S6" t="s">
         <v>403</v>
       </c>
-      <c r="T6" t="s">
+      <c r="V6" t="s">
         <v>362</v>
       </c>
-      <c r="V6" t="s">
+      <c r="X6" t="s">
         <v>98</v>
       </c>
-      <c r="W6" t="s">
+      <c r="Y6" t="s">
         <v>515</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Z6" t="s">
         <v>180</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="AA6" t="s">
         <v>186</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AB6" t="s">
         <v>520</v>
       </c>
-      <c r="AA6" t="s">
-        <v>233</v>
+      <c r="AC6" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
         <v>378</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>225</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>367</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>524</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>16</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>316</v>
       </c>
-      <c r="N7" t="s">
+      <c r="P7" t="s">
         <v>33</v>
       </c>
-      <c r="O7" t="s">
+      <c r="Q7" t="s">
         <v>245</v>
       </c>
-      <c r="P7" t="s">
+      <c r="R7" t="s">
         <v>502</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="S7" t="s">
         <v>404</v>
       </c>
-      <c r="T7" t="s">
+      <c r="V7" t="s">
         <v>361</v>
       </c>
-      <c r="V7" t="s">
+      <c r="X7" t="s">
         <v>99</v>
       </c>
-      <c r="W7" t="s">
+      <c r="Y7" t="s">
         <v>516</v>
       </c>
-      <c r="X7" t="s">
+      <c r="Z7" t="s">
         <v>181</v>
       </c>
-      <c r="Y7" t="s">
+      <c r="AA7" t="s">
         <v>187</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="AB7" t="s">
         <v>521</v>
       </c>
-      <c r="AA7" t="s">
-        <v>234</v>
+      <c r="AC7" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
         <v>379</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>319</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>368</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>329</v>
       </c>
-      <c r="J8" t="s">
-        <v>79</v>
-      </c>
-      <c r="L8" t="s">
+      <c r="K8" t="s">
+        <v>559</v>
+      </c>
+      <c r="M8" t="s">
         <v>34</v>
       </c>
-      <c r="N8" t="s">
+      <c r="P8" t="s">
         <v>90</v>
       </c>
-      <c r="O8" t="s">
+      <c r="Q8" t="s">
         <v>246</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="S8" t="s">
         <v>405</v>
       </c>
-      <c r="T8" t="s">
+      <c r="V8" t="s">
         <v>363</v>
       </c>
-      <c r="V8" t="s">
+      <c r="X8" t="s">
         <v>100</v>
       </c>
-      <c r="W8" t="s">
+      <c r="Y8" t="s">
         <v>175</v>
       </c>
-      <c r="X8" t="s">
+      <c r="Z8" t="s">
         <v>182</v>
       </c>
-      <c r="Y8" t="s">
+      <c r="AA8" t="s">
         <v>188</v>
       </c>
-      <c r="Z8" t="s">
+      <c r="AB8" t="s">
         <v>522</v>
       </c>
-      <c r="AA8" t="s">
-        <v>235</v>
+      <c r="AC8" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>348</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
         <v>380</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>32</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>307</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>330</v>
       </c>
-      <c r="J9" t="s">
-        <v>38</v>
-      </c>
-      <c r="L9" t="s">
+      <c r="K9" t="s">
+        <v>79</v>
+      </c>
+      <c r="M9" t="s">
         <v>35</v>
       </c>
-      <c r="N9" t="s">
+      <c r="P9" t="s">
         <v>91</v>
       </c>
-      <c r="O9" t="s">
+      <c r="Q9" t="s">
         <v>247</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="S9" t="s">
         <v>406</v>
       </c>
-      <c r="T9" t="s">
+      <c r="V9" t="s">
         <v>364</v>
       </c>
-      <c r="V9" t="s">
+      <c r="X9" t="s">
         <v>210</v>
       </c>
-      <c r="Y9" t="s">
+      <c r="AA9" t="s">
         <v>189</v>
       </c>
-      <c r="AA9" t="s">
-        <v>236</v>
+      <c r="AC9" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" t="s">
+        <v>348</v>
+      </c>
+      <c r="E10" t="s">
         <v>316</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>353</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>535</v>
       </c>
-      <c r="J10" t="s">
-        <v>391</v>
-      </c>
-      <c r="L10" t="s">
+      <c r="K10" t="s">
+        <v>38</v>
+      </c>
+      <c r="M10" t="s">
         <v>36</v>
       </c>
-      <c r="N10" t="s">
+      <c r="P10" t="s">
         <v>501</v>
       </c>
-      <c r="O10" t="s">
+      <c r="Q10" t="s">
         <v>248</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="S10" t="s">
         <v>407</v>
       </c>
-      <c r="V10" t="s">
+      <c r="X10" t="s">
         <v>258</v>
       </c>
-      <c r="Y10" t="s">
+      <c r="AA10" t="s">
         <v>190</v>
       </c>
-      <c r="AA10" t="s">
-        <v>237</v>
+      <c r="AC10" t="s">
+        <v>577</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>334</v>
-      </c>
-      <c r="D11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" t="s">
         <v>256</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>275</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>323</v>
       </c>
-      <c r="J11" t="s">
-        <v>17</v>
-      </c>
-      <c r="L11" t="s">
-        <v>497</v>
-      </c>
-      <c r="N11" t="s">
+      <c r="K11" t="s">
+        <v>560</v>
+      </c>
+      <c r="M11" t="s">
+        <v>562</v>
+      </c>
+      <c r="P11" t="s">
         <v>92</v>
       </c>
-      <c r="O11" t="s">
+      <c r="Q11" t="s">
         <v>249</v>
       </c>
-      <c r="V11" t="s">
+      <c r="X11" t="s">
         <v>259</v>
       </c>
-      <c r="Y11" t="s">
+      <c r="AA11" t="s">
         <v>260</v>
       </c>
-      <c r="AA11" t="s">
-        <v>238</v>
+      <c r="AC11" t="s">
+        <v>578</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" t="s">
+        <v>334</v>
+      </c>
+      <c r="E12" t="s">
         <v>320</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>264</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>324</v>
       </c>
-      <c r="J12" t="s">
-        <v>42</v>
-      </c>
-      <c r="L12" t="s">
-        <v>39</v>
-      </c>
-      <c r="N12" t="s">
+      <c r="K12" t="s">
+        <v>391</v>
+      </c>
+      <c r="M12" t="s">
+        <v>497</v>
+      </c>
+      <c r="P12" t="s">
         <v>41</v>
       </c>
-      <c r="O12" t="s">
+      <c r="Q12" t="s">
         <v>250</v>
       </c>
-      <c r="V12" t="s">
+      <c r="X12" t="s">
         <v>101</v>
       </c>
-      <c r="Y12" t="s">
+      <c r="AA12" t="s">
         <v>191</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>579</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>196</v>
-      </c>
-      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" t="s">
         <v>342</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>317</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>325</v>
       </c>
-      <c r="J13" t="s">
-        <v>80</v>
-      </c>
-      <c r="L13" t="s">
-        <v>40</v>
-      </c>
-      <c r="N13" t="s">
+      <c r="K13" t="s">
+        <v>17</v>
+      </c>
+      <c r="M13" t="s">
+        <v>563</v>
+      </c>
+      <c r="P13" t="s">
         <v>93</v>
       </c>
-      <c r="O13" t="s">
+      <c r="Q13" t="s">
         <v>255</v>
       </c>
-      <c r="V13" t="s">
+      <c r="X13" t="s">
         <v>327</v>
       </c>
-      <c r="Y13" t="s">
+      <c r="AA13" t="s">
         <v>192</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>580</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>51</v>
-      </c>
-      <c r="D14" t="s">
+        <v>549</v>
+      </c>
+      <c r="E14" t="s">
         <v>37</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>265</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>326</v>
       </c>
-      <c r="J14" t="s">
-        <v>81</v>
-      </c>
-      <c r="L14" t="s">
-        <v>43</v>
-      </c>
-      <c r="N14" t="s">
+      <c r="K14" t="s">
+        <v>42</v>
+      </c>
+      <c r="M14" t="s">
+        <v>39</v>
+      </c>
+      <c r="P14" t="s">
         <v>94</v>
       </c>
-      <c r="O14" t="s">
+      <c r="Q14" t="s">
         <v>251</v>
       </c>
-      <c r="V14" t="s">
+      <c r="X14" t="s">
         <v>102</v>
       </c>
-      <c r="Y14" t="s">
+      <c r="AA14" t="s">
         <v>193</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>581</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>240</v>
-      </c>
-      <c r="D15" t="s">
+        <v>196</v>
+      </c>
+      <c r="E15" t="s">
         <v>58</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>266</v>
       </c>
-      <c r="J15" t="s">
-        <v>538</v>
-      </c>
-      <c r="N15" t="s">
-        <v>95</v>
-      </c>
-      <c r="O15" t="s">
+      <c r="K15" t="s">
+        <v>561</v>
+      </c>
+      <c r="M15" t="s">
+        <v>40</v>
+      </c>
+      <c r="P15" t="s">
+        <v>567</v>
+      </c>
+      <c r="Q15" t="s">
         <v>252</v>
       </c>
-      <c r="V15" t="s">
+      <c r="X15" t="s">
         <v>103</v>
       </c>
-      <c r="Y15" t="s">
+      <c r="AA15" t="s">
         <v>194</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>582</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" t="s">
         <v>386</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>318</v>
       </c>
-      <c r="J16" t="s">
-        <v>82</v>
-      </c>
-      <c r="O16" t="s">
+      <c r="K16" t="s">
+        <v>80</v>
+      </c>
+      <c r="M16" t="s">
+        <v>43</v>
+      </c>
+      <c r="P16" t="s">
+        <v>568</v>
+      </c>
+      <c r="Q16" t="s">
         <v>253</v>
       </c>
-      <c r="V16" t="s">
+      <c r="X16" t="s">
         <v>74</v>
       </c>
-      <c r="Y16" t="s">
+      <c r="AA16" t="s">
         <v>195</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>583</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>397</v>
-      </c>
-      <c r="D17" t="s">
+        <v>240</v>
+      </c>
+      <c r="E17" t="s">
         <v>387</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>88</v>
       </c>
-      <c r="J17" t="s">
-        <v>83</v>
-      </c>
-      <c r="V17" t="s">
-        <v>104</v>
-      </c>
-      <c r="Y17" t="s">
+      <c r="K17" t="s">
+        <v>81</v>
+      </c>
+      <c r="X17" t="s">
+        <v>569</v>
+      </c>
+      <c r="AA17" t="s">
         <v>543</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>584</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>488</v>
-      </c>
-      <c r="D18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" t="s">
         <v>491</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>89</v>
       </c>
-      <c r="J18" t="s">
-        <v>381</v>
-      </c>
-      <c r="V18" t="s">
-        <v>105</v>
+      <c r="K18" t="s">
+        <v>538</v>
+      </c>
+      <c r="X18" t="s">
+        <v>104</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>585</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>489</v>
-      </c>
-      <c r="D19" t="s">
+        <v>397</v>
+      </c>
+      <c r="E19" t="s">
         <v>59</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>297</v>
       </c>
-      <c r="J19" t="s">
-        <v>547</v>
-      </c>
-      <c r="V19" t="s">
-        <v>106</v>
+      <c r="K19" t="s">
+        <v>82</v>
+      </c>
+      <c r="X19" t="s">
+        <v>105</v>
+      </c>
+      <c r="AC19" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>358</v>
-      </c>
-      <c r="D20" t="s">
+        <v>488</v>
+      </c>
+      <c r="E20" t="s">
         <v>60</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>298</v>
       </c>
-      <c r="J20" t="s">
-        <v>44</v>
-      </c>
-      <c r="V20" t="s">
-        <v>107</v>
+      <c r="K20" t="s">
+        <v>83</v>
+      </c>
+      <c r="X20" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC20" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>398</v>
-      </c>
-      <c r="D21" t="s">
+        <v>489</v>
+      </c>
+      <c r="E21" t="s">
         <v>257</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>299</v>
       </c>
-      <c r="J21" t="s">
-        <v>393</v>
-      </c>
-      <c r="V21" t="s">
-        <v>108</v>
+      <c r="K21" t="s">
+        <v>381</v>
+      </c>
+      <c r="X21" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" t="s">
+        <v>358</v>
+      </c>
+      <c r="E22" t="s">
         <v>61</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>300</v>
       </c>
-      <c r="J22" t="s">
-        <v>84</v>
-      </c>
-      <c r="V22" t="s">
-        <v>109</v>
+      <c r="K22" t="s">
+        <v>547</v>
+      </c>
+      <c r="X22" t="s">
+        <v>570</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>54</v>
-      </c>
-      <c r="D23" t="s">
+        <v>398</v>
+      </c>
+      <c r="E23" t="s">
         <v>322</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>291</v>
       </c>
-      <c r="J23" t="s">
-        <v>495</v>
-      </c>
-      <c r="V23" t="s">
-        <v>110</v>
+      <c r="K23" t="s">
+        <v>44</v>
+      </c>
+      <c r="X23" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>55</v>
-      </c>
-      <c r="D24" t="s">
+        <v>53</v>
+      </c>
+      <c r="E24" t="s">
         <v>62</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>280</v>
       </c>
-      <c r="J24" t="s">
-        <v>45</v>
-      </c>
-      <c r="V24" t="s">
-        <v>111</v>
+      <c r="K24" t="s">
+        <v>393</v>
+      </c>
+      <c r="X24" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>56</v>
-      </c>
-      <c r="D25" t="s">
+        <v>54</v>
+      </c>
+      <c r="E25" t="s">
         <v>530</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>75</v>
       </c>
-      <c r="J25" t="s">
-        <v>46</v>
-      </c>
-      <c r="V25" t="s">
-        <v>112</v>
+      <c r="K25" t="s">
+        <v>84</v>
+      </c>
+      <c r="X25" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>490</v>
-      </c>
-      <c r="D26" t="s">
+        <v>55</v>
+      </c>
+      <c r="E26" t="s">
         <v>226</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>283</v>
       </c>
-      <c r="V26" t="s">
-        <v>113</v>
+      <c r="K26" t="s">
+        <v>495</v>
+      </c>
+      <c r="X26" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
+        <v>56</v>
+      </c>
+      <c r="E27" t="s">
+        <v>227</v>
+      </c>
+      <c r="G27" t="s">
+        <v>267</v>
+      </c>
+      <c r="K27" t="s">
+        <v>45</v>
+      </c>
+      <c r="X27" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>490</v>
+      </c>
+      <c r="E28" t="s">
+        <v>544</v>
+      </c>
+      <c r="G28" t="s">
+        <v>284</v>
+      </c>
+      <c r="K28" t="s">
+        <v>46</v>
+      </c>
+      <c r="X28" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
         <v>228</v>
       </c>
-      <c r="D27" t="s">
-        <v>227</v>
-      </c>
-      <c r="F27" t="s">
-        <v>267</v>
-      </c>
-      <c r="V27" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="D28" t="s">
-        <v>544</v>
-      </c>
-      <c r="F28" t="s">
-        <v>284</v>
-      </c>
-      <c r="V28" t="s">
+      <c r="E29" t="s">
+        <v>545</v>
+      </c>
+      <c r="G29" t="s">
+        <v>285</v>
+      </c>
+      <c r="X29" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="29">
-      <c r="D29" t="s">
-        <v>545</v>
-      </c>
-      <c r="F29" t="s">
-        <v>285</v>
-      </c>
-      <c r="V29" t="s">
+    <row r="30">
+      <c r="E30" t="s">
+        <v>492</v>
+      </c>
+      <c r="G30" t="s">
+        <v>217</v>
+      </c>
+      <c r="X30" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="30">
-      <c r="D30" t="s">
-        <v>492</v>
-      </c>
-      <c r="F30" t="s">
-        <v>217</v>
-      </c>
-      <c r="V30" t="s">
+    <row r="31">
+      <c r="E31" t="s">
+        <v>63</v>
+      </c>
+      <c r="G31" t="s">
+        <v>276</v>
+      </c>
+      <c r="X31" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="31">
-      <c r="D31" t="s">
-        <v>63</v>
-      </c>
-      <c r="F31" t="s">
-        <v>276</v>
-      </c>
-      <c r="V31" t="s">
+    <row r="32">
+      <c r="E32" t="s">
+        <v>64</v>
+      </c>
+      <c r="G32" t="s">
+        <v>286</v>
+      </c>
+      <c r="X32" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="32">
-      <c r="D32" t="s">
-        <v>64</v>
-      </c>
-      <c r="F32" t="s">
-        <v>286</v>
-      </c>
-      <c r="V32" t="s">
+    <row r="33">
+      <c r="E33" t="s">
+        <v>65</v>
+      </c>
+      <c r="G33" t="s">
+        <v>555</v>
+      </c>
+      <c r="X33" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="33">
-      <c r="D33" t="s">
-        <v>65</v>
-      </c>
-      <c r="F33" t="s">
+    <row r="34">
+      <c r="E34" t="s">
+        <v>66</v>
+      </c>
+      <c r="G34" t="s">
         <v>261</v>
       </c>
-      <c r="V33" t="s">
+      <c r="X34" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="34">
-      <c r="D34" t="s">
-        <v>66</v>
-      </c>
-      <c r="F34" t="s">
+    <row r="35">
+      <c r="E35" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" t="s">
         <v>331</v>
       </c>
-      <c r="V34" t="s">
+      <c r="X35" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="35">
-      <c r="D35" t="s">
-        <v>67</v>
-      </c>
-      <c r="F35" t="s">
+    <row r="36">
+      <c r="E36" t="s">
+        <v>68</v>
+      </c>
+      <c r="G36" t="s">
         <v>308</v>
       </c>
-      <c r="V35" t="s">
+      <c r="X36" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="36">
-      <c r="D36" t="s">
-        <v>68</v>
-      </c>
-      <c r="F36" t="s">
+    <row r="37">
+      <c r="E37" t="s">
+        <v>69</v>
+      </c>
+      <c r="G37" t="s">
         <v>262</v>
       </c>
-      <c r="V36" t="s">
+      <c r="X37" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="37">
-      <c r="D37" t="s">
-        <v>69</v>
-      </c>
-      <c r="F37" t="s">
+    <row r="38">
+      <c r="E38" t="s">
+        <v>70</v>
+      </c>
+      <c r="G38" t="s">
         <v>309</v>
       </c>
-      <c r="V37" t="s">
+      <c r="X38" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="38">
-      <c r="D38" t="s">
-        <v>70</v>
-      </c>
-      <c r="F38" t="s">
+    <row r="39">
+      <c r="G39" t="s">
         <v>268</v>
       </c>
-      <c r="V38" t="s">
+      <c r="X39" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="39">
-      <c r="F39" t="s">
+    <row r="40">
+      <c r="G40" t="s">
         <v>77</v>
       </c>
-      <c r="V39" t="s">
+      <c r="X40" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="40">
-      <c r="F40" t="s">
+    <row r="41">
+      <c r="G41" t="s">
         <v>213</v>
       </c>
-      <c r="V40" t="s">
+      <c r="X41" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="41">
-      <c r="F41" t="s">
+    <row r="42">
+      <c r="G42" t="s">
         <v>290</v>
       </c>
-      <c r="V41" t="s">
+      <c r="X42" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="42">
-      <c r="F42" t="s">
+    <row r="43">
+      <c r="G43" t="s">
         <v>301</v>
       </c>
-      <c r="V42" t="s">
+      <c r="X43" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="43">
-      <c r="F43" t="s">
+    <row r="44">
+      <c r="G44" t="s">
         <v>302</v>
       </c>
-      <c r="V43" t="s">
+      <c r="X44" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="44">
-      <c r="F44" t="s">
+    <row r="45">
+      <c r="G45" t="s">
         <v>344</v>
       </c>
-      <c r="V44" t="s">
+      <c r="X45" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="45">
-      <c r="F45" t="s">
+    <row r="46">
+      <c r="G46" t="s">
         <v>343</v>
       </c>
-      <c r="V45" t="s">
+      <c r="X46" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="46">
-      <c r="F46" t="s">
+    <row r="47">
+      <c r="G47" t="s">
         <v>212</v>
       </c>
-      <c r="V46" t="s">
+      <c r="X47" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="47">
-      <c r="F47" t="s">
+    <row r="48">
+      <c r="G48" t="s">
         <v>321</v>
       </c>
-      <c r="V47" t="s">
+      <c r="X48" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="48">
-      <c r="F48" t="s">
+    <row r="49">
+      <c r="G49" t="s">
         <v>340</v>
       </c>
-      <c r="V48" t="s">
+      <c r="X49" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="49">
-      <c r="F49" t="s">
+    <row r="50">
+      <c r="G50" t="s">
         <v>369</v>
       </c>
-      <c r="V49" t="s">
+      <c r="X50" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="50">
-      <c r="F50" t="s">
+    <row r="51">
+      <c r="G51" t="s">
         <v>303</v>
       </c>
-      <c r="V50" t="s">
+      <c r="X51" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="51">
-      <c r="F51" t="s">
+    <row r="52">
+      <c r="G52" t="s">
         <v>357</v>
       </c>
-      <c r="V51" t="s">
+      <c r="X52" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="G53" t="s">
+        <v>332</v>
+      </c>
+      <c r="X53" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="52">
-      <c r="F52" t="s">
-        <v>332</v>
-      </c>
-      <c r="V52" t="s">
+    <row r="54">
+      <c r="G54" t="s">
+        <v>269</v>
+      </c>
+      <c r="X54" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="53">
-      <c r="F53" t="s">
-        <v>269</v>
-      </c>
-      <c r="V53" t="s">
+    <row r="55">
+      <c r="G55" t="s">
+        <v>293</v>
+      </c>
+      <c r="X55" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="54">
-      <c r="F54" t="s">
-        <v>293</v>
-      </c>
-      <c r="V54" t="s">
+    <row r="56">
+      <c r="G56" t="s">
+        <v>294</v>
+      </c>
+      <c r="X56" t="s">
         <v>540</v>
       </c>
     </row>
-    <row r="55">
-      <c r="F55" t="s">
-        <v>294</v>
-      </c>
-      <c r="V55" t="s">
+    <row r="57">
+      <c r="G57" t="s">
+        <v>295</v>
+      </c>
+      <c r="X57" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="56">
-      <c r="F56" t="s">
-        <v>295</v>
-      </c>
-      <c r="V56" t="s">
+    <row r="58">
+      <c r="G58" t="s">
+        <v>304</v>
+      </c>
+      <c r="X58" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="57">
-      <c r="F57" t="s">
-        <v>304</v>
-      </c>
-      <c r="V57" t="s">
+    <row r="59">
+      <c r="G59" t="s">
+        <v>313</v>
+      </c>
+      <c r="X59" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="58">
-      <c r="F58" t="s">
-        <v>313</v>
-      </c>
-      <c r="V58" t="s">
+    <row r="60">
+      <c r="G60" t="s">
+        <v>338</v>
+      </c>
+      <c r="X60" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="59">
-      <c r="F59" t="s">
-        <v>338</v>
-      </c>
-      <c r="V59" t="s">
+    <row r="61">
+      <c r="G61" t="s">
+        <v>310</v>
+      </c>
+      <c r="X61" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="60">
-      <c r="F60" t="s">
-        <v>310</v>
-      </c>
-      <c r="V60" t="s">
+    <row r="62">
+      <c r="G62" t="s">
+        <v>311</v>
+      </c>
+      <c r="X62" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="61">
-      <c r="F61" t="s">
-        <v>311</v>
-      </c>
-      <c r="V61" t="s">
+    <row r="63">
+      <c r="G63" t="s">
+        <v>370</v>
+      </c>
+      <c r="X63" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="62">
-      <c r="F62" t="s">
-        <v>370</v>
-      </c>
-      <c r="V62" t="s">
+    <row r="64">
+      <c r="G64" t="s">
+        <v>371</v>
+      </c>
+      <c r="X64" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="63">
-      <c r="F63" t="s">
-        <v>371</v>
-      </c>
-      <c r="V63" t="s">
+    <row r="65">
+      <c r="G65" t="s">
+        <v>346</v>
+      </c>
+      <c r="X65" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="G66" t="s">
+        <v>314</v>
+      </c>
+      <c r="X66" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="64">
-      <c r="F64" t="s">
-        <v>346</v>
-      </c>
-      <c r="V64" t="s">
+    <row r="67">
+      <c r="G67" t="s">
+        <v>270</v>
+      </c>
+      <c r="X67" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="65">
-      <c r="F65" t="s">
-        <v>314</v>
-      </c>
-      <c r="V65" t="s">
+    <row r="68">
+      <c r="G68" t="s">
+        <v>354</v>
+      </c>
+      <c r="X68" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="66">
-      <c r="F66" t="s">
-        <v>270</v>
-      </c>
-      <c r="V66" t="s">
+    <row r="69">
+      <c r="G69" t="s">
+        <v>315</v>
+      </c>
+      <c r="X69" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="67">
-      <c r="F67" t="s">
-        <v>354</v>
-      </c>
-      <c r="V67" t="s">
+    <row r="70">
+      <c r="G70" t="s">
+        <v>411</v>
+      </c>
+      <c r="X70" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="68">
-      <c r="F68" t="s">
-        <v>315</v>
-      </c>
-      <c r="V68" t="s">
+    <row r="71">
+      <c r="G71" t="s">
+        <v>305</v>
+      </c>
+      <c r="X71" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="69">
-      <c r="F69" t="s">
-        <v>411</v>
-      </c>
-      <c r="V69" t="s">
+    <row r="72">
+      <c r="G72" t="s">
+        <v>412</v>
+      </c>
+      <c r="X72" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="70">
-      <c r="F70" t="s">
-        <v>305</v>
-      </c>
-      <c r="V70" t="s">
+    <row r="73">
+      <c r="G73" t="s">
+        <v>263</v>
+      </c>
+      <c r="X73" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="71">
-      <c r="F71" t="s">
-        <v>412</v>
-      </c>
-      <c r="V71" t="s">
+    <row r="74">
+      <c r="G74" t="s">
+        <v>556</v>
+      </c>
+      <c r="X74" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="72">
-      <c r="F72" t="s">
-        <v>263</v>
-      </c>
-      <c r="V72" t="s">
+    <row r="75">
+      <c r="G75" t="s">
+        <v>345</v>
+      </c>
+      <c r="X75" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="73">
-      <c r="F73" t="s">
-        <v>345</v>
-      </c>
-      <c r="V73" t="s">
+    <row r="76">
+      <c r="G76" t="s">
+        <v>281</v>
+      </c>
+      <c r="X76" t="s">
         <v>546</v>
       </c>
     </row>
-    <row r="74">
-      <c r="F74" t="s">
-        <v>281</v>
-      </c>
-      <c r="V74" t="s">
+    <row r="77">
+      <c r="G77" t="s">
+        <v>287</v>
+      </c>
+      <c r="X77" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="75">
-      <c r="F75" t="s">
-        <v>287</v>
-      </c>
-      <c r="V75" t="s">
+    <row r="78">
+      <c r="G78" t="s">
+        <v>292</v>
+      </c>
+      <c r="X78" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="76">
-      <c r="F76" t="s">
-        <v>292</v>
-      </c>
-      <c r="V76" t="s">
+    <row r="79">
+      <c r="G79" t="s">
+        <v>494</v>
+      </c>
+      <c r="X79" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="77">
-      <c r="F77" t="s">
-        <v>494</v>
-      </c>
-      <c r="V77" t="s">
+    <row r="80">
+      <c r="G80" t="s">
+        <v>333</v>
+      </c>
+      <c r="X80" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="G81" t="s">
+        <v>271</v>
+      </c>
+      <c r="X81" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="78">
-      <c r="F78" t="s">
-        <v>333</v>
-      </c>
-      <c r="V78" t="s">
+    <row r="82">
+      <c r="G82" t="s">
+        <v>282</v>
+      </c>
+      <c r="X82" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="79">
-      <c r="F79" t="s">
-        <v>271</v>
-      </c>
-      <c r="V79" t="s">
+    <row r="83">
+      <c r="G83" t="s">
+        <v>288</v>
+      </c>
+      <c r="X83" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="80">
-      <c r="F80" t="s">
-        <v>282</v>
-      </c>
-      <c r="V80" t="s">
+    <row r="84">
+      <c r="G84" t="s">
+        <v>277</v>
+      </c>
+      <c r="X84" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="G85" t="s">
+        <v>272</v>
+      </c>
+      <c r="X85" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="81">
-      <c r="F81" t="s">
-        <v>288</v>
-      </c>
-      <c r="V81" t="s">
+    <row r="86">
+      <c r="G86" t="s">
+        <v>289</v>
+      </c>
+      <c r="X86" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="82">
-      <c r="F82" t="s">
-        <v>277</v>
-      </c>
-      <c r="V82" t="s">
+    <row r="87">
+      <c r="G87" t="s">
+        <v>273</v>
+      </c>
+      <c r="X87" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="83">
-      <c r="F83" t="s">
-        <v>272</v>
-      </c>
-      <c r="V83" t="s">
+    <row r="88">
+      <c r="G88" t="s">
+        <v>274</v>
+      </c>
+      <c r="X88" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="84">
-      <c r="F84" t="s">
-        <v>289</v>
-      </c>
-      <c r="V84" t="s">
+    <row r="89">
+      <c r="G89" t="s">
+        <v>306</v>
+      </c>
+      <c r="X89" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="85">
-      <c r="F85" t="s">
-        <v>273</v>
-      </c>
-      <c r="V85" t="s">
+    <row r="90">
+      <c r="G90" t="s">
+        <v>312</v>
+      </c>
+      <c r="X90" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="86">
-      <c r="F86" t="s">
-        <v>274</v>
-      </c>
-      <c r="V86" t="s">
+    <row r="91">
+      <c r="G91" t="s">
+        <v>296</v>
+      </c>
+      <c r="X91" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="87">
-      <c r="F87" t="s">
-        <v>306</v>
-      </c>
-      <c r="V87" t="s">
+    <row r="92">
+      <c r="G92" t="s">
+        <v>341</v>
+      </c>
+      <c r="X92" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="88">
-      <c r="F88" t="s">
-        <v>312</v>
-      </c>
-      <c r="V88" t="s">
+    <row r="93">
+      <c r="G93" t="s">
+        <v>278</v>
+      </c>
+      <c r="X93" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="89">
-      <c r="F89" t="s">
-        <v>296</v>
-      </c>
-      <c r="V89" t="s">
+    <row r="94">
+      <c r="G94" t="s">
+        <v>279</v>
+      </c>
+      <c r="X94" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="90">
-      <c r="F90" t="s">
-        <v>341</v>
-      </c>
-      <c r="V90" t="s">
+    <row r="95">
+      <c r="X95" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="91">
-      <c r="F91" t="s">
-        <v>278</v>
-      </c>
-      <c r="V91" t="s">
+    <row r="96">
+      <c r="X96" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="92">
-      <c r="F92" t="s">
-        <v>279</v>
-      </c>
-      <c r="V92" t="s">
+    <row r="97">
+      <c r="X97" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="93">
-      <c r="V93" t="s">
+    <row r="98">
+      <c r="X98" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="94">
-      <c r="V94" t="s">
+    <row r="99">
+      <c r="X99" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="95">
-      <c r="V95" t="s">
+    <row r="100">
+      <c r="X100" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="X101" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="96">
-      <c r="V96" t="s">
+    <row r="102">
+      <c r="X102" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="97">
-      <c r="V97" t="s">
+    <row r="103">
+      <c r="X103" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="98">
-      <c r="V98" t="s">
+    <row r="104">
+      <c r="X104" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="99">
-      <c r="V99" t="s">
+    <row r="105">
+      <c r="X105" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="100">
-      <c r="V100" t="s">
+    <row r="106">
+      <c r="X106" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="101">
-      <c r="V101" t="s">
+    <row r="107">
+      <c r="X107" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="102">
-      <c r="V102" t="s">
+    <row r="108">
+      <c r="X108" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="103">
-      <c r="V103" t="s">
+    <row r="109">
+      <c r="X109" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="104">
-      <c r="V104" t="s">
+    <row r="110">
+      <c r="X110" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="105">
-      <c r="V105" t="s">
+    <row r="111">
+      <c r="X111" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="106">
-      <c r="V106" t="s">
+    <row r="112">
+      <c r="X112" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="107">
-      <c r="V107" t="s">
+    <row r="113">
+      <c r="X113" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="108">
-      <c r="V108" t="s">
+    <row r="114">
+      <c r="X114" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="109">
-      <c r="V109" t="s">
+    <row r="115">
+      <c r="X115" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="110">
-      <c r="V110" t="s">
+    <row r="116">
+      <c r="X116" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="111">
-      <c r="V111" t="s">
+    <row r="117">
+      <c r="X117" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="112">
-      <c r="V112" t="s">
+    <row r="118">
+      <c r="X118" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="113">
-      <c r="V113" t="s">
+    <row r="119">
+      <c r="X119" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="114">
-      <c r="V114" t="s">
+    <row r="120">
+      <c r="X120" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="115">
-      <c r="V115" t="s">
+    <row r="121">
+      <c r="X121" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="116">
-      <c r="V116" t="s">
+    <row r="122">
+      <c r="X122" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="117">
-      <c r="V117" t="s">
+    <row r="123">
+      <c r="X123" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="118">
-      <c r="V118" t="s">
+    <row r="124">
+      <c r="X124" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="119">
-      <c r="V119" t="s">
+    <row r="125">
+      <c r="X125" t="s">
         <v>170</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- **NEW** command type to create, maintain and manipulate a local-only relational database. One can use such facility   to collect execution-bound data over multiple executions, or use the SQL capability to manipulate structured data set   of any conceivable size.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/demo1/artifact/script/InjestData.xlsx
+++ b/demo1/artifact/script/InjestData.xlsx
@@ -31,28 +31,29 @@
     <definedName name="io">'#system'!$K$2:$K$28</definedName>
     <definedName name="jms">'#system'!$L$2:$L$4</definedName>
     <definedName name="json">'#system'!$M$2:$M$16</definedName>
-    <definedName name="mail">'#system'!$O$2:$O$2</definedName>
+    <definedName name="mail">'#system'!$P$2:$P$2</definedName>
     <definedName name="math">'#system'!$K$2:$K$13</definedName>
     <definedName name="mq">'#system'!$J$2:$J$3</definedName>
     <definedName name="nextgen">'#system'!$K$2:$K$28</definedName>
-    <definedName name="number">'#system'!$P$2:$P$16</definedName>
-    <definedName name="pdf">'#system'!$Q$2:$Q$16</definedName>
-    <definedName name="rdbms">'#system'!$R$2:$R$7</definedName>
-    <definedName name="redis">'#system'!$S$2:$S$10</definedName>
-    <definedName name="ssh">'#system'!$V$2:$V$9</definedName>
-    <definedName name="step">'#system'!$W$2:$W$4</definedName>
-    <definedName name="target">'#system'!$A$2:$A$29</definedName>
-    <definedName name="web">'#system'!$X$2:$X$125</definedName>
-    <definedName name="webalert">'#system'!$Y$2:$Y$8</definedName>
-    <definedName name="webcookie">'#system'!$Z$2:$Z$8</definedName>
-    <definedName name="ws">'#system'!$AA$2:$AA$17</definedName>
-    <definedName name="xml">'#system'!$AC$2:$AC$21</definedName>
-    <definedName name="sms">'#system'!$T$2:$T$2</definedName>
-    <definedName name="sound">'#system'!$U$2:$U$5</definedName>
-    <definedName name="ws.async">'#system'!$AB$2:$AB$8</definedName>
+    <definedName name="number">'#system'!$Q$2:$Q$16</definedName>
+    <definedName name="pdf">'#system'!$R$2:$R$16</definedName>
+    <definedName name="rdbms">'#system'!$S$2:$S$7</definedName>
+    <definedName name="redis">'#system'!$T$2:$T$10</definedName>
+    <definedName name="ssh">'#system'!$W$2:$W$9</definedName>
+    <definedName name="step">'#system'!$X$2:$X$4</definedName>
+    <definedName name="target">'#system'!$A$2:$A$30</definedName>
+    <definedName name="web">'#system'!$Y$2:$Y$127</definedName>
+    <definedName name="webalert">'#system'!$Z$2:$Z$8</definedName>
+    <definedName name="webcookie">'#system'!$AA$2:$AA$8</definedName>
+    <definedName name="ws">'#system'!$AB$2:$AB$17</definedName>
+    <definedName name="xml">'#system'!$AD$2:$AD$21</definedName>
+    <definedName name="sms">'#system'!$U$2:$U$2</definedName>
+    <definedName name="sound">'#system'!$V$2:$V$5</definedName>
+    <definedName name="ws.async">'#system'!$AC$2:$AC$8</definedName>
     <definedName name="aws.ses">'#system'!$C$2:$C$3</definedName>
     <definedName name="aws.sqs">'#system'!$D$2:$D$5</definedName>
-    <definedName name="macro">'#system'!$N$2:$N$4</definedName>
+    <definedName name="macro">'#system'!$O$2:$O$4</definedName>
+    <definedName name="localdb">'#system'!$N$2:$N$7</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
@@ -72,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3988" uniqueCount="586">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4516" uniqueCount="595">
   <si>
     <t>description</t>
   </si>
@@ -1831,6 +1832,33 @@
   </si>
   <si>
     <t>replaceIn(xml,xpath,content,var)</t>
+  </si>
+  <si>
+    <t>localdb</t>
+  </si>
+  <si>
+    <t>cloneTable(var,source,target)</t>
+  </si>
+  <si>
+    <t>dropTables(var,tables)</t>
+  </si>
+  <si>
+    <t>exportCSV(sql,output)</t>
+  </si>
+  <si>
+    <t>importRecords(var,sourceDb,sql,table)</t>
+  </si>
+  <si>
+    <t>purge(var)</t>
+  </si>
+  <si>
+    <t>runSQLs(var,sqls)</t>
+  </si>
+  <si>
+    <t>scrollElement(locator,xOffset,yOffset)</t>
+  </si>
+  <si>
+    <t>scrollPage(xOffset,yOffset)</t>
   </si>
 </sst>
 </file>
@@ -1838,7 +1866,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="123" x14ac:knownFonts="1">
+  <fonts count="139" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2622,8 +2650,109 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="823C3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="194">
+  <fills count="224">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3719,8 +3848,178 @@
         <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="202">
+  <borders count="230">
     <border>
       <left/>
       <right/>
@@ -5769,6 +6068,288 @@
         <color rgb="C3C3C3"/>
       </bottom>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
@@ -5776,7 +6357,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="154">
+  <cellXfs count="170">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="2" fontId="7" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -6215,52 +6796,100 @@
     <xf applyFont="true" borderId="0" fillId="0" fontId="106" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="107" fillId="169" borderId="181" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="181" fillId="169" fontId="107" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="108" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="108" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="109" fillId="172" borderId="185" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="185" fillId="172" fontId="109" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="110" fillId="175" borderId="189" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="189" fillId="175" fontId="110" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="111" fillId="178" borderId="189" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="189" fillId="178" fontId="111" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="112" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="112" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="113" fillId="181" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="181" fontId="113" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="114" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="114" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="115" fillId="184" borderId="193" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="193" fillId="184" fontId="115" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="116" fillId="187" borderId="197" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="197" fillId="187" fontId="116" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="117" fillId="190" borderId="201" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="201" fillId="190" fontId="117" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="118" fillId="190" borderId="201" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="201" fillId="190" fontId="118" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="119" fillId="178" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="178" fontId="119" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="120" fillId="193" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="193" fontId="120" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="121" fillId="178" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="178" fontId="121" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="122" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="122" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="123" fillId="196" borderId="209" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="124" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="125" fillId="199" borderId="213" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="126" fillId="202" borderId="217" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="127" fillId="205" borderId="217" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="128" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="129" fillId="208" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="130" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="131" fillId="211" borderId="221" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="132" fillId="214" borderId="225" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="133" fillId="217" borderId="229" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="134" fillId="217" borderId="229" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="135" fillId="205" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="136" fillId="220" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="137" fillId="205" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="138" fillId="223" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -6645,7 +7274,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD125"/>
+  <dimension ref="A1:AE127"/>
   <sheetViews>
     <sheetView tabSelected="false" workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125">
       <selection activeCell="A19" sqref="A19"/>
@@ -6697,51 +7326,54 @@
         <v>24</v>
       </c>
       <c r="N1" t="s">
+        <v>586</v>
+      </c>
+      <c r="O1" t="s">
         <v>549</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>196</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>51</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>240</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>52</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>397</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>488</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>489</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>358</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>398</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>53</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>54</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>55</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>56</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>490</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>228</v>
       </c>
     </row>
@@ -6786,51 +7418,54 @@
         <v>496</v>
       </c>
       <c r="N2" t="s">
+        <v>587</v>
+      </c>
+      <c r="O2" t="s">
         <v>564</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>498</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>499</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>254</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>218</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>399</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>503</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>504</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>382</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>408</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>96</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>171</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>176</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>183</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>517</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>576</v>
       </c>
     </row>
@@ -6875,45 +7510,48 @@
         <v>85</v>
       </c>
       <c r="N3" t="s">
+        <v>588</v>
+      </c>
+      <c r="O3" t="s">
         <v>565</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>500</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>241</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>219</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>400</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>505</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>383</v>
       </c>
-      <c r="W3" t="s">
+      <c r="X3" t="s">
         <v>409</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>97</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
         <v>172</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AA3" t="s">
         <v>177</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AB3" t="s">
         <v>365</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AC3" t="s">
         <v>184</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AD3" t="s">
         <v>229</v>
       </c>
     </row>
@@ -6955,45 +7593,48 @@
         <v>25</v>
       </c>
       <c r="N4" t="s">
+        <v>589</v>
+      </c>
+      <c r="O4" t="s">
         <v>566</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>26</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>242</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>220</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>401</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>506</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>359</v>
       </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
         <v>410</v>
       </c>
-      <c r="X4" t="s">
+      <c r="Y4" t="s">
         <v>355</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="Z4" t="s">
         <v>173</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AA4" t="s">
         <v>178</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AB4" t="s">
         <v>184</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AC4" t="s">
         <v>518</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AD4" t="s">
         <v>230</v>
       </c>
     </row>
@@ -7028,40 +7669,43 @@
       <c r="M5" t="s">
         <v>86</v>
       </c>
-      <c r="P5" t="s">
+      <c r="N5" t="s">
+        <v>590</v>
+      </c>
+      <c r="Q5" t="s">
         <v>30</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>243</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>221</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>402</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>507</v>
       </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
         <v>360</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Y5" t="s">
         <v>356</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="Z5" t="s">
         <v>174</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AA5" t="s">
         <v>179</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AB5" t="s">
         <v>185</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AC5" t="s">
         <v>519</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AD5" t="s">
         <v>231</v>
       </c>
     </row>
@@ -7093,37 +7737,40 @@
       <c r="M6" t="s">
         <v>29</v>
       </c>
-      <c r="P6" t="s">
+      <c r="N6" t="s">
+        <v>591</v>
+      </c>
+      <c r="Q6" t="s">
         <v>31</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>244</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>392</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>403</v>
       </c>
-      <c r="V6" t="s">
+      <c r="W6" t="s">
         <v>362</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Y6" t="s">
         <v>98</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="Z6" t="s">
         <v>515</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AA6" t="s">
         <v>180</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AB6" t="s">
         <v>186</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AC6" t="s">
         <v>520</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AD6" t="s">
         <v>232</v>
       </c>
     </row>
@@ -7149,37 +7796,40 @@
       <c r="M7" t="s">
         <v>316</v>
       </c>
-      <c r="P7" t="s">
+      <c r="N7" t="s">
+        <v>592</v>
+      </c>
+      <c r="Q7" t="s">
         <v>33</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="R7" t="s">
         <v>245</v>
       </c>
-      <c r="R7" t="s">
+      <c r="S7" t="s">
         <v>502</v>
       </c>
-      <c r="S7" t="s">
+      <c r="T7" t="s">
         <v>404</v>
       </c>
-      <c r="V7" t="s">
+      <c r="W7" t="s">
         <v>361</v>
       </c>
-      <c r="X7" t="s">
+      <c r="Y7" t="s">
         <v>99</v>
       </c>
-      <c r="Y7" t="s">
+      <c r="Z7" t="s">
         <v>516</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="AA7" t="s">
         <v>181</v>
       </c>
-      <c r="AA7" t="s">
+      <c r="AB7" t="s">
         <v>187</v>
       </c>
-      <c r="AB7" t="s">
+      <c r="AC7" t="s">
         <v>521</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="AD7" t="s">
         <v>233</v>
       </c>
     </row>
@@ -7205,34 +7855,34 @@
       <c r="M8" t="s">
         <v>34</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>90</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="R8" t="s">
         <v>246</v>
       </c>
-      <c r="S8" t="s">
+      <c r="T8" t="s">
         <v>405</v>
       </c>
-      <c r="V8" t="s">
+      <c r="W8" t="s">
         <v>363</v>
       </c>
-      <c r="X8" t="s">
+      <c r="Y8" t="s">
         <v>100</v>
       </c>
-      <c r="Y8" t="s">
+      <c r="Z8" t="s">
         <v>175</v>
       </c>
-      <c r="Z8" t="s">
+      <c r="AA8" t="s">
         <v>182</v>
       </c>
-      <c r="AA8" t="s">
+      <c r="AB8" t="s">
         <v>188</v>
       </c>
-      <c r="AB8" t="s">
+      <c r="AC8" t="s">
         <v>522</v>
       </c>
-      <c r="AC8" t="s">
+      <c r="AD8" t="s">
         <v>234</v>
       </c>
     </row>
@@ -7258,25 +7908,25 @@
       <c r="M9" t="s">
         <v>35</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>91</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="R9" t="s">
         <v>247</v>
       </c>
-      <c r="S9" t="s">
+      <c r="T9" t="s">
         <v>406</v>
       </c>
-      <c r="V9" t="s">
+      <c r="W9" t="s">
         <v>364</v>
       </c>
-      <c r="X9" t="s">
+      <c r="Y9" t="s">
         <v>210</v>
       </c>
-      <c r="AA9" t="s">
+      <c r="AB9" t="s">
         <v>189</v>
       </c>
-      <c r="AC9" t="s">
+      <c r="AD9" t="s">
         <v>235</v>
       </c>
     </row>
@@ -7299,22 +7949,22 @@
       <c r="M10" t="s">
         <v>36</v>
       </c>
-      <c r="P10" t="s">
+      <c r="Q10" t="s">
         <v>501</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="R10" t="s">
         <v>248</v>
       </c>
-      <c r="S10" t="s">
+      <c r="T10" t="s">
         <v>407</v>
       </c>
-      <c r="X10" t="s">
+      <c r="Y10" t="s">
         <v>258</v>
       </c>
-      <c r="AA10" t="s">
+      <c r="AB10" t="s">
         <v>190</v>
       </c>
-      <c r="AC10" t="s">
+      <c r="AD10" t="s">
         <v>577</v>
       </c>
     </row>
@@ -7337,19 +7987,19 @@
       <c r="M11" t="s">
         <v>562</v>
       </c>
-      <c r="P11" t="s">
+      <c r="Q11" t="s">
         <v>92</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="R11" t="s">
         <v>249</v>
       </c>
-      <c r="X11" t="s">
+      <c r="Y11" t="s">
         <v>259</v>
       </c>
-      <c r="AA11" t="s">
+      <c r="AB11" t="s">
         <v>260</v>
       </c>
-      <c r="AC11" t="s">
+      <c r="AD11" t="s">
         <v>578</v>
       </c>
     </row>
@@ -7372,19 +8022,19 @@
       <c r="M12" t="s">
         <v>497</v>
       </c>
-      <c r="P12" t="s">
+      <c r="Q12" t="s">
         <v>41</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="R12" t="s">
         <v>250</v>
       </c>
-      <c r="X12" t="s">
+      <c r="Y12" t="s">
         <v>101</v>
       </c>
-      <c r="AA12" t="s">
+      <c r="AB12" t="s">
         <v>191</v>
       </c>
-      <c r="AC12" t="s">
+      <c r="AD12" t="s">
         <v>579</v>
       </c>
     </row>
@@ -7407,25 +8057,25 @@
       <c r="M13" t="s">
         <v>563</v>
       </c>
-      <c r="P13" t="s">
+      <c r="Q13" t="s">
         <v>93</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="R13" t="s">
         <v>255</v>
       </c>
-      <c r="X13" t="s">
+      <c r="Y13" t="s">
         <v>327</v>
       </c>
-      <c r="AA13" t="s">
+      <c r="AB13" t="s">
         <v>192</v>
       </c>
-      <c r="AC13" t="s">
+      <c r="AD13" t="s">
         <v>580</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>549</v>
+        <v>586</v>
       </c>
       <c r="E14" t="s">
         <v>37</v>
@@ -7442,25 +8092,25 @@
       <c r="M14" t="s">
         <v>39</v>
       </c>
-      <c r="P14" t="s">
+      <c r="Q14" t="s">
         <v>94</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="R14" t="s">
         <v>251</v>
       </c>
-      <c r="X14" t="s">
+      <c r="Y14" t="s">
         <v>102</v>
       </c>
-      <c r="AA14" t="s">
+      <c r="AB14" t="s">
         <v>193</v>
       </c>
-      <c r="AC14" t="s">
+      <c r="AD14" t="s">
         <v>581</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>196</v>
+        <v>549</v>
       </c>
       <c r="E15" t="s">
         <v>58</v>
@@ -7474,25 +8124,25 @@
       <c r="M15" t="s">
         <v>40</v>
       </c>
-      <c r="P15" t="s">
+      <c r="Q15" t="s">
         <v>567</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="R15" t="s">
         <v>252</v>
       </c>
-      <c r="X15" t="s">
+      <c r="Y15" t="s">
         <v>103</v>
       </c>
-      <c r="AA15" t="s">
+      <c r="AB15" t="s">
         <v>194</v>
       </c>
-      <c r="AC15" t="s">
+      <c r="AD15" t="s">
         <v>582</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>196</v>
       </c>
       <c r="E16" t="s">
         <v>386</v>
@@ -7506,25 +8156,25 @@
       <c r="M16" t="s">
         <v>43</v>
       </c>
-      <c r="P16" t="s">
+      <c r="Q16" t="s">
         <v>568</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="R16" t="s">
         <v>253</v>
       </c>
-      <c r="X16" t="s">
+      <c r="Y16" t="s">
         <v>74</v>
       </c>
-      <c r="AA16" t="s">
+      <c r="AB16" t="s">
         <v>195</v>
       </c>
-      <c r="AC16" t="s">
+      <c r="AD16" t="s">
         <v>583</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>240</v>
+        <v>51</v>
       </c>
       <c r="E17" t="s">
         <v>387</v>
@@ -7535,19 +8185,19 @@
       <c r="K17" t="s">
         <v>81</v>
       </c>
-      <c r="X17" t="s">
+      <c r="Y17" t="s">
         <v>569</v>
       </c>
-      <c r="AA17" t="s">
+      <c r="AB17" t="s">
         <v>543</v>
       </c>
-      <c r="AC17" t="s">
+      <c r="AD17" t="s">
         <v>584</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>240</v>
       </c>
       <c r="E18" t="s">
         <v>491</v>
@@ -7558,16 +8208,16 @@
       <c r="K18" t="s">
         <v>538</v>
       </c>
-      <c r="X18" t="s">
+      <c r="Y18" t="s">
         <v>104</v>
       </c>
-      <c r="AC18" t="s">
+      <c r="AD18" t="s">
         <v>585</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>397</v>
+        <v>52</v>
       </c>
       <c r="E19" t="s">
         <v>59</v>
@@ -7578,16 +8228,16 @@
       <c r="K19" t="s">
         <v>82</v>
       </c>
-      <c r="X19" t="s">
+      <c r="Y19" t="s">
         <v>105</v>
       </c>
-      <c r="AC19" t="s">
+      <c r="AD19" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>488</v>
+        <v>397</v>
       </c>
       <c r="E20" t="s">
         <v>60</v>
@@ -7598,16 +8248,16 @@
       <c r="K20" t="s">
         <v>83</v>
       </c>
-      <c r="X20" t="s">
+      <c r="Y20" t="s">
         <v>106</v>
       </c>
-      <c r="AC20" t="s">
+      <c r="AD20" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="E21" t="s">
         <v>257</v>
@@ -7618,16 +8268,16 @@
       <c r="K21" t="s">
         <v>381</v>
       </c>
-      <c r="X21" t="s">
+      <c r="Y21" t="s">
         <v>107</v>
       </c>
-      <c r="AC21" t="s">
+      <c r="AD21" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>358</v>
+        <v>489</v>
       </c>
       <c r="E22" t="s">
         <v>61</v>
@@ -7638,13 +8288,13 @@
       <c r="K22" t="s">
         <v>547</v>
       </c>
-      <c r="X22" t="s">
+      <c r="Y22" t="s">
         <v>570</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>398</v>
+        <v>358</v>
       </c>
       <c r="E23" t="s">
         <v>322</v>
@@ -7655,13 +8305,13 @@
       <c r="K23" t="s">
         <v>44</v>
       </c>
-      <c r="X23" t="s">
+      <c r="Y23" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>398</v>
       </c>
       <c r="E24" t="s">
         <v>62</v>
@@ -7672,13 +8322,13 @@
       <c r="K24" t="s">
         <v>393</v>
       </c>
-      <c r="X24" t="s">
+      <c r="Y24" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E25" t="s">
         <v>530</v>
@@ -7689,13 +8339,13 @@
       <c r="K25" t="s">
         <v>84</v>
       </c>
-      <c r="X25" t="s">
+      <c r="Y25" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E26" t="s">
         <v>226</v>
@@ -7706,13 +8356,13 @@
       <c r="K26" t="s">
         <v>495</v>
       </c>
-      <c r="X26" t="s">
+      <c r="Y26" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E27" t="s">
         <v>227</v>
@@ -7723,13 +8373,13 @@
       <c r="K27" t="s">
         <v>45</v>
       </c>
-      <c r="X27" t="s">
+      <c r="Y27" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>490</v>
+        <v>56</v>
       </c>
       <c r="E28" t="s">
         <v>544</v>
@@ -7740,13 +8390,13 @@
       <c r="K28" t="s">
         <v>46</v>
       </c>
-      <c r="X28" t="s">
+      <c r="Y28" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>228</v>
+        <v>490</v>
       </c>
       <c r="E29" t="s">
         <v>545</v>
@@ -7754,18 +8404,21 @@
       <c r="G29" t="s">
         <v>285</v>
       </c>
-      <c r="X29" t="s">
+      <c r="Y29" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="30">
+      <c r="A30" t="s">
+        <v>228</v>
+      </c>
       <c r="E30" t="s">
         <v>492</v>
       </c>
       <c r="G30" t="s">
         <v>217</v>
       </c>
-      <c r="X30" t="s">
+      <c r="Y30" t="s">
         <v>115</v>
       </c>
     </row>
@@ -7776,7 +8429,7 @@
       <c r="G31" t="s">
         <v>276</v>
       </c>
-      <c r="X31" t="s">
+      <c r="Y31" t="s">
         <v>116</v>
       </c>
     </row>
@@ -7787,7 +8440,7 @@
       <c r="G32" t="s">
         <v>286</v>
       </c>
-      <c r="X32" t="s">
+      <c r="Y32" t="s">
         <v>117</v>
       </c>
     </row>
@@ -7798,7 +8451,7 @@
       <c r="G33" t="s">
         <v>555</v>
       </c>
-      <c r="X33" t="s">
+      <c r="Y33" t="s">
         <v>118</v>
       </c>
     </row>
@@ -7809,7 +8462,7 @@
       <c r="G34" t="s">
         <v>261</v>
       </c>
-      <c r="X34" t="s">
+      <c r="Y34" t="s">
         <v>119</v>
       </c>
     </row>
@@ -7820,7 +8473,7 @@
       <c r="G35" t="s">
         <v>331</v>
       </c>
-      <c r="X35" t="s">
+      <c r="Y35" t="s">
         <v>211</v>
       </c>
     </row>
@@ -7831,7 +8484,7 @@
       <c r="G36" t="s">
         <v>308</v>
       </c>
-      <c r="X36" t="s">
+      <c r="Y36" t="s">
         <v>120</v>
       </c>
     </row>
@@ -7842,7 +8495,7 @@
       <c r="G37" t="s">
         <v>262</v>
       </c>
-      <c r="X37" t="s">
+      <c r="Y37" t="s">
         <v>339</v>
       </c>
     </row>
@@ -7853,7 +8506,7 @@
       <c r="G38" t="s">
         <v>309</v>
       </c>
-      <c r="X38" t="s">
+      <c r="Y38" t="s">
         <v>508</v>
       </c>
     </row>
@@ -7861,7 +8514,7 @@
       <c r="G39" t="s">
         <v>268</v>
       </c>
-      <c r="X39" t="s">
+      <c r="Y39" t="s">
         <v>394</v>
       </c>
     </row>
@@ -7869,7 +8522,7 @@
       <c r="G40" t="s">
         <v>77</v>
       </c>
-      <c r="X40" t="s">
+      <c r="Y40" t="s">
         <v>121</v>
       </c>
     </row>
@@ -7877,7 +8530,7 @@
       <c r="G41" t="s">
         <v>213</v>
       </c>
-      <c r="X41" t="s">
+      <c r="Y41" t="s">
         <v>122</v>
       </c>
     </row>
@@ -7885,7 +8538,7 @@
       <c r="G42" t="s">
         <v>290</v>
       </c>
-      <c r="X42" t="s">
+      <c r="Y42" t="s">
         <v>123</v>
       </c>
     </row>
@@ -7893,7 +8546,7 @@
       <c r="G43" t="s">
         <v>301</v>
       </c>
-      <c r="X43" t="s">
+      <c r="Y43" t="s">
         <v>124</v>
       </c>
     </row>
@@ -7901,7 +8554,7 @@
       <c r="G44" t="s">
         <v>302</v>
       </c>
-      <c r="X44" t="s">
+      <c r="Y44" t="s">
         <v>125</v>
       </c>
     </row>
@@ -7909,7 +8562,7 @@
       <c r="G45" t="s">
         <v>344</v>
       </c>
-      <c r="X45" t="s">
+      <c r="Y45" t="s">
         <v>126</v>
       </c>
     </row>
@@ -7917,7 +8570,7 @@
       <c r="G46" t="s">
         <v>343</v>
       </c>
-      <c r="X46" t="s">
+      <c r="Y46" t="s">
         <v>509</v>
       </c>
     </row>
@@ -7925,7 +8578,7 @@
       <c r="G47" t="s">
         <v>212</v>
       </c>
-      <c r="X47" t="s">
+      <c r="Y47" t="s">
         <v>214</v>
       </c>
     </row>
@@ -7933,7 +8586,7 @@
       <c r="G48" t="s">
         <v>321</v>
       </c>
-      <c r="X48" t="s">
+      <c r="Y48" t="s">
         <v>76</v>
       </c>
     </row>
@@ -7941,7 +8594,7 @@
       <c r="G49" t="s">
         <v>340</v>
       </c>
-      <c r="X49" t="s">
+      <c r="Y49" t="s">
         <v>127</v>
       </c>
     </row>
@@ -7949,7 +8602,7 @@
       <c r="G50" t="s">
         <v>369</v>
       </c>
-      <c r="X50" t="s">
+      <c r="Y50" t="s">
         <v>128</v>
       </c>
     </row>
@@ -7957,7 +8610,7 @@
       <c r="G51" t="s">
         <v>303</v>
       </c>
-      <c r="X51" t="s">
+      <c r="Y51" t="s">
         <v>129</v>
       </c>
     </row>
@@ -7965,7 +8618,7 @@
       <c r="G52" t="s">
         <v>357</v>
       </c>
-      <c r="X52" t="s">
+      <c r="Y52" t="s">
         <v>571</v>
       </c>
     </row>
@@ -7973,7 +8626,7 @@
       <c r="G53" t="s">
         <v>332</v>
       </c>
-      <c r="X53" t="s">
+      <c r="Y53" t="s">
         <v>539</v>
       </c>
     </row>
@@ -7981,7 +8634,7 @@
       <c r="G54" t="s">
         <v>269</v>
       </c>
-      <c r="X54" t="s">
+      <c r="Y54" t="s">
         <v>130</v>
       </c>
     </row>
@@ -7989,7 +8642,7 @@
       <c r="G55" t="s">
         <v>293</v>
       </c>
-      <c r="X55" t="s">
+      <c r="Y55" t="s">
         <v>347</v>
       </c>
     </row>
@@ -7997,7 +8650,7 @@
       <c r="G56" t="s">
         <v>294</v>
       </c>
-      <c r="X56" t="s">
+      <c r="Y56" t="s">
         <v>540</v>
       </c>
     </row>
@@ -8005,7 +8658,7 @@
       <c r="G57" t="s">
         <v>295</v>
       </c>
-      <c r="X57" t="s">
+      <c r="Y57" t="s">
         <v>131</v>
       </c>
     </row>
@@ -8013,7 +8666,7 @@
       <c r="G58" t="s">
         <v>304</v>
       </c>
-      <c r="X58" t="s">
+      <c r="Y58" t="s">
         <v>132</v>
       </c>
     </row>
@@ -8021,7 +8674,7 @@
       <c r="G59" t="s">
         <v>313</v>
       </c>
-      <c r="X59" t="s">
+      <c r="Y59" t="s">
         <v>133</v>
       </c>
     </row>
@@ -8029,7 +8682,7 @@
       <c r="G60" t="s">
         <v>338</v>
       </c>
-      <c r="X60" t="s">
+      <c r="Y60" t="s">
         <v>134</v>
       </c>
     </row>
@@ -8037,7 +8690,7 @@
       <c r="G61" t="s">
         <v>310</v>
       </c>
-      <c r="X61" t="s">
+      <c r="Y61" t="s">
         <v>135</v>
       </c>
     </row>
@@ -8045,7 +8698,7 @@
       <c r="G62" t="s">
         <v>311</v>
       </c>
-      <c r="X62" t="s">
+      <c r="Y62" t="s">
         <v>136</v>
       </c>
     </row>
@@ -8053,7 +8706,7 @@
       <c r="G63" t="s">
         <v>370</v>
       </c>
-      <c r="X63" t="s">
+      <c r="Y63" t="s">
         <v>137</v>
       </c>
     </row>
@@ -8061,7 +8714,7 @@
       <c r="G64" t="s">
         <v>371</v>
       </c>
-      <c r="X64" t="s">
+      <c r="Y64" t="s">
         <v>510</v>
       </c>
     </row>
@@ -8069,7 +8722,7 @@
       <c r="G65" t="s">
         <v>346</v>
       </c>
-      <c r="X65" t="s">
+      <c r="Y65" t="s">
         <v>572</v>
       </c>
     </row>
@@ -8077,7 +8730,7 @@
       <c r="G66" t="s">
         <v>314</v>
       </c>
-      <c r="X66" t="s">
+      <c r="Y66" t="s">
         <v>215</v>
       </c>
     </row>
@@ -8085,7 +8738,7 @@
       <c r="G67" t="s">
         <v>270</v>
       </c>
-      <c r="X67" t="s">
+      <c r="Y67" t="s">
         <v>390</v>
       </c>
     </row>
@@ -8093,7 +8746,7 @@
       <c r="G68" t="s">
         <v>354</v>
       </c>
-      <c r="X68" t="s">
+      <c r="Y68" t="s">
         <v>511</v>
       </c>
     </row>
@@ -8101,7 +8754,7 @@
       <c r="G69" t="s">
         <v>315</v>
       </c>
-      <c r="X69" t="s">
+      <c r="Y69" t="s">
         <v>138</v>
       </c>
     </row>
@@ -8109,7 +8762,7 @@
       <c r="G70" t="s">
         <v>411</v>
       </c>
-      <c r="X70" t="s">
+      <c r="Y70" t="s">
         <v>139</v>
       </c>
     </row>
@@ -8117,7 +8770,7 @@
       <c r="G71" t="s">
         <v>305</v>
       </c>
-      <c r="X71" t="s">
+      <c r="Y71" t="s">
         <v>140</v>
       </c>
     </row>
@@ -8125,7 +8778,7 @@
       <c r="G72" t="s">
         <v>412</v>
       </c>
-      <c r="X72" t="s">
+      <c r="Y72" t="s">
         <v>141</v>
       </c>
     </row>
@@ -8133,7 +8786,7 @@
       <c r="G73" t="s">
         <v>263</v>
       </c>
-      <c r="X73" t="s">
+      <c r="Y73" t="s">
         <v>198</v>
       </c>
     </row>
@@ -8141,7 +8794,7 @@
       <c r="G74" t="s">
         <v>556</v>
       </c>
-      <c r="X74" t="s">
+      <c r="Y74" t="s">
         <v>199</v>
       </c>
     </row>
@@ -8149,7 +8802,7 @@
       <c r="G75" t="s">
         <v>345</v>
       </c>
-      <c r="X75" t="s">
+      <c r="Y75" t="s">
         <v>541</v>
       </c>
     </row>
@@ -8157,7 +8810,7 @@
       <c r="G76" t="s">
         <v>281</v>
       </c>
-      <c r="X76" t="s">
+      <c r="Y76" t="s">
         <v>546</v>
       </c>
     </row>
@@ -8165,7 +8818,7 @@
       <c r="G77" t="s">
         <v>287</v>
       </c>
-      <c r="X77" t="s">
+      <c r="Y77" t="s">
         <v>142</v>
       </c>
     </row>
@@ -8173,7 +8826,7 @@
       <c r="G78" t="s">
         <v>292</v>
       </c>
-      <c r="X78" t="s">
+      <c r="Y78" t="s">
         <v>143</v>
       </c>
     </row>
@@ -8181,7 +8834,7 @@
       <c r="G79" t="s">
         <v>494</v>
       </c>
-      <c r="X79" t="s">
+      <c r="Y79" t="s">
         <v>144</v>
       </c>
     </row>
@@ -8189,7 +8842,7 @@
       <c r="G80" t="s">
         <v>333</v>
       </c>
-      <c r="X80" t="s">
+      <c r="Y80" t="s">
         <v>573</v>
       </c>
     </row>
@@ -8197,7 +8850,7 @@
       <c r="G81" t="s">
         <v>271</v>
       </c>
-      <c r="X81" t="s">
+      <c r="Y81" t="s">
         <v>145</v>
       </c>
     </row>
@@ -8205,7 +8858,7 @@
       <c r="G82" t="s">
         <v>282</v>
       </c>
-      <c r="X82" t="s">
+      <c r="Y82" t="s">
         <v>146</v>
       </c>
     </row>
@@ -8213,7 +8866,7 @@
       <c r="G83" t="s">
         <v>288</v>
       </c>
-      <c r="X83" t="s">
+      <c r="Y83" t="s">
         <v>200</v>
       </c>
     </row>
@@ -8221,7 +8874,7 @@
       <c r="G84" t="s">
         <v>277</v>
       </c>
-      <c r="X84" t="s">
+      <c r="Y84" t="s">
         <v>574</v>
       </c>
     </row>
@@ -8229,7 +8882,7 @@
       <c r="G85" t="s">
         <v>272</v>
       </c>
-      <c r="X85" t="s">
+      <c r="Y85" t="s">
         <v>201</v>
       </c>
     </row>
@@ -8237,7 +8890,7 @@
       <c r="G86" t="s">
         <v>289</v>
       </c>
-      <c r="X86" t="s">
+      <c r="Y86" t="s">
         <v>542</v>
       </c>
     </row>
@@ -8245,7 +8898,7 @@
       <c r="G87" t="s">
         <v>273</v>
       </c>
-      <c r="X87" t="s">
+      <c r="Y87" t="s">
         <v>202</v>
       </c>
     </row>
@@ -8253,7 +8906,7 @@
       <c r="G88" t="s">
         <v>274</v>
       </c>
-      <c r="X88" t="s">
+      <c r="Y88" t="s">
         <v>203</v>
       </c>
     </row>
@@ -8261,7 +8914,7 @@
       <c r="G89" t="s">
         <v>306</v>
       </c>
-      <c r="X89" t="s">
+      <c r="Y89" t="s">
         <v>216</v>
       </c>
     </row>
@@ -8269,7 +8922,7 @@
       <c r="G90" t="s">
         <v>312</v>
       </c>
-      <c r="X90" t="s">
+      <c r="Y90" t="s">
         <v>147</v>
       </c>
     </row>
@@ -8277,7 +8930,7 @@
       <c r="G91" t="s">
         <v>296</v>
       </c>
-      <c r="X91" t="s">
+      <c r="Y91" t="s">
         <v>204</v>
       </c>
     </row>
@@ -8285,7 +8938,7 @@
       <c r="G92" t="s">
         <v>341</v>
       </c>
-      <c r="X92" t="s">
+      <c r="Y92" t="s">
         <v>512</v>
       </c>
     </row>
@@ -8293,7 +8946,7 @@
       <c r="G93" t="s">
         <v>278</v>
       </c>
-      <c r="X93" t="s">
+      <c r="Y93" t="s">
         <v>513</v>
       </c>
     </row>
@@ -8301,162 +8954,172 @@
       <c r="G94" t="s">
         <v>279</v>
       </c>
-      <c r="X94" t="s">
+      <c r="Y94" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="95">
-      <c r="X95" t="s">
+      <c r="Y95" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="96">
-      <c r="X96" t="s">
+      <c r="Y96" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="97">
-      <c r="X97" t="s">
+      <c r="Y97" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="98">
-      <c r="X98" t="s">
+      <c r="Y98" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="99">
-      <c r="X99" t="s">
+      <c r="Y99" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="100">
-      <c r="X100" t="s">
+      <c r="Y100" t="s">
         <v>575</v>
       </c>
     </row>
     <row r="101">
-      <c r="X101" t="s">
+      <c r="Y101" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="Y102" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="102">
-      <c r="X102" t="s">
+    <row r="103">
+      <c r="Y103" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="Y104" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="103">
-      <c r="X103" t="s">
+    <row r="105">
+      <c r="Y105" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="104">
-      <c r="X104" t="s">
+    <row r="106">
+      <c r="Y106" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="105">
-      <c r="X105" t="s">
+    <row r="107">
+      <c r="Y107" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="106">
-      <c r="X106" t="s">
+    <row r="108">
+      <c r="Y108" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="107">
-      <c r="X107" t="s">
+    <row r="109">
+      <c r="Y109" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="108">
-      <c r="X108" t="s">
+    <row r="110">
+      <c r="Y110" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="109">
-      <c r="X109" t="s">
+    <row r="111">
+      <c r="Y111" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="110">
-      <c r="X110" t="s">
+    <row r="112">
+      <c r="Y112" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="111">
-      <c r="X111" t="s">
+    <row r="113">
+      <c r="Y113" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="112">
-      <c r="X112" t="s">
+    <row r="114">
+      <c r="Y114" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="113">
-      <c r="X113" t="s">
+    <row r="115">
+      <c r="Y115" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="114">
-      <c r="X114" t="s">
+    <row r="116">
+      <c r="Y116" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="115">
-      <c r="X115" t="s">
+    <row r="117">
+      <c r="Y117" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="116">
-      <c r="X116" t="s">
+    <row r="118">
+      <c r="Y118" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="117">
-      <c r="X117" t="s">
+    <row r="119">
+      <c r="Y119" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="118">
-      <c r="X118" t="s">
+    <row r="120">
+      <c r="Y120" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="119">
-      <c r="X119" t="s">
+    <row r="121">
+      <c r="Y121" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="120">
-      <c r="X120" t="s">
+    <row r="122">
+      <c r="Y122" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="121">
-      <c r="X121" t="s">
+    <row r="123">
+      <c r="Y123" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="122">
-      <c r="X122" t="s">
+    <row r="124">
+      <c r="Y124" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="123">
-      <c r="X123" t="s">
+    <row r="125">
+      <c r="Y125" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="124">
-      <c r="X124" t="s">
+    <row r="126">
+      <c r="Y126" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="125">
-      <c r="X125" t="s">
+    <row r="127">
+      <c r="Y127" t="s">
         <v>170</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added demo project for Nov. 19 Meetup
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/demo1/artifact/script/InjestData.xlsx
+++ b/demo1/artifact/script/InjestData.xlsx
@@ -20,13 +20,13 @@
   </sheets>
   <definedNames>
     <definedName name="aws.s3">'#system'!$B$2:$B$9</definedName>
-    <definedName name="base">'#system'!$F$2:$F$40</definedName>
+    <definedName name="base">'#system'!$F$2:$F$39</definedName>
     <definedName name="csv">'#system'!$G$2:$G$6</definedName>
     <definedName name="date">'#system'!$C$2:$C$14</definedName>
     <definedName name="db">'#system'!$D$2:$D$5</definedName>
     <definedName name="desktop">'#system'!$H$2:$H$98</definedName>
     <definedName name="excel">'#system'!$I$2:$I$14</definedName>
-    <definedName name="external">'#system'!$J$2:$J$5</definedName>
+    <definedName name="external">'#system'!$J$2:$J$6</definedName>
     <definedName name="image">'#system'!$K$2:$K$7</definedName>
     <definedName name="io">'#system'!$L$2:$L$30</definedName>
     <definedName name="jms">'#system'!$M$2:$M$4</definedName>
@@ -42,7 +42,7 @@
     <definedName name="ssh">'#system'!$X$2:$X$9</definedName>
     <definedName name="step">'#system'!$Y$2:$Y$4</definedName>
     <definedName name="target">'#system'!$A$2:$A$31</definedName>
-    <definedName name="web">'#system'!$Z$2:$Z$135</definedName>
+    <definedName name="web">'#system'!$Z$2:$Z$137</definedName>
     <definedName name="webalert">'#system'!$AA$2:$AA$8</definedName>
     <definedName name="webcookie">'#system'!$AB$2:$AB$8</definedName>
     <definedName name="ws">'#system'!$AC$2:$AC$17</definedName>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5613" uniqueCount="635">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6178" uniqueCount="638">
   <si>
     <t>description</t>
   </si>
@@ -1980,6 +1980,15 @@
   </si>
   <si>
     <t>storeSoapFaultString(var,xml)</t>
+  </si>
+  <si>
+    <t>terminate(programName)</t>
+  </si>
+  <si>
+    <t>saveSelectedText(var,locator)</t>
+  </si>
+  <si>
+    <t>saveSelectedValue(var,locator)</t>
   </si>
 </sst>
 </file>
@@ -1987,7 +1996,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="171" x14ac:knownFonts="1">
+  <fonts count="187" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3074,8 +3083,109 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="281">
+  <fills count="308">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4664,8 +4774,161 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="290">
+  <borders count="322">
     <border>
       <left/>
       <right/>
@@ -7604,6 +7867,332 @@
         <color rgb="C3C3C3"/>
       </bottom>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
@@ -7611,7 +8200,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="202">
+  <cellXfs count="218">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="2" fontId="7" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -8194,52 +8783,100 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="253" fontId="154" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="155" fillId="256" borderId="265" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="265" fillId="256" fontId="155" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="156" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="156" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="157" fillId="259" borderId="269" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="269" fillId="259" fontId="157" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="158" fillId="262" borderId="273" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="273" fillId="262" fontId="158" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="159" fillId="265" borderId="277" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="277" fillId="265" fontId="159" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="160" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="160" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="161" fillId="268" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="268" fontId="161" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="162" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="162" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="163" fillId="271" borderId="281" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="281" fillId="271" fontId="163" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="164" fillId="262" borderId="285" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="285" fillId="262" fontId="164" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="165" fillId="274" borderId="289" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="289" fillId="274" fontId="165" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="166" fillId="274" borderId="289" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="289" fillId="274" fontId="166" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="167" fillId="265" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="265" fontId="167" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="168" fillId="277" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="277" fontId="168" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="169" fillId="265" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="265" fontId="169" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="170" fillId="280" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="280" fontId="170" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="171" fillId="283" borderId="297" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="172" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="173" fillId="286" borderId="301" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="174" fillId="289" borderId="305" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="175" fillId="292" borderId="309" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="176" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="177" fillId="295" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="178" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="179" fillId="298" borderId="313" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="180" fillId="289" borderId="317" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="181" fillId="301" borderId="321" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="182" fillId="301" borderId="321" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="183" fillId="292" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="184" fillId="304" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="185" fillId="292" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="186" fillId="307" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -8624,7 +9261,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF135"/>
+  <dimension ref="A1:AF137"/>
   <sheetViews>
     <sheetView tabSelected="false" workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125">
       <selection activeCell="A19" sqref="A19"/>
@@ -9090,6 +9727,9 @@
       <c r="I6" t="s">
         <v>534</v>
       </c>
+      <c r="J6" t="s">
+        <v>635</v>
+      </c>
       <c r="K6" t="s">
         <v>349</v>
       </c>
@@ -9606,7 +10246,7 @@
         <v>240</v>
       </c>
       <c r="F19" t="s">
-        <v>603</v>
+        <v>59</v>
       </c>
       <c r="H19" t="s">
         <v>89</v>
@@ -9626,7 +10266,7 @@
         <v>52</v>
       </c>
       <c r="F20" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H20" t="s">
         <v>297</v>
@@ -9646,7 +10286,7 @@
         <v>397</v>
       </c>
       <c r="F21" t="s">
-        <v>60</v>
+        <v>257</v>
       </c>
       <c r="H21" t="s">
         <v>298</v>
@@ -9666,7 +10306,7 @@
         <v>488</v>
       </c>
       <c r="F22" t="s">
-        <v>257</v>
+        <v>604</v>
       </c>
       <c r="H22" t="s">
         <v>299</v>
@@ -9686,7 +10326,7 @@
         <v>489</v>
       </c>
       <c r="F23" t="s">
-        <v>604</v>
+        <v>61</v>
       </c>
       <c r="H23" t="s">
         <v>300</v>
@@ -9706,7 +10346,7 @@
         <v>358</v>
       </c>
       <c r="F24" t="s">
-        <v>61</v>
+        <v>322</v>
       </c>
       <c r="H24" t="s">
         <v>291</v>
@@ -9726,7 +10366,7 @@
         <v>398</v>
       </c>
       <c r="F25" t="s">
-        <v>322</v>
+        <v>62</v>
       </c>
       <c r="H25" t="s">
         <v>280</v>
@@ -9746,7 +10386,7 @@
         <v>53</v>
       </c>
       <c r="F26" t="s">
-        <v>62</v>
+        <v>530</v>
       </c>
       <c r="H26" t="s">
         <v>75</v>
@@ -9766,7 +10406,7 @@
         <v>54</v>
       </c>
       <c r="F27" t="s">
-        <v>530</v>
+        <v>226</v>
       </c>
       <c r="H27" t="s">
         <v>283</v>
@@ -9786,7 +10426,7 @@
         <v>55</v>
       </c>
       <c r="F28" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H28" t="s">
         <v>267</v>
@@ -9803,7 +10443,7 @@
         <v>56</v>
       </c>
       <c r="F29" t="s">
-        <v>227</v>
+        <v>544</v>
       </c>
       <c r="H29" t="s">
         <v>284</v>
@@ -9820,7 +10460,7 @@
         <v>490</v>
       </c>
       <c r="F30" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="H30" t="s">
         <v>285</v>
@@ -9837,7 +10477,7 @@
         <v>228</v>
       </c>
       <c r="F31" t="s">
-        <v>545</v>
+        <v>492</v>
       </c>
       <c r="H31" t="s">
         <v>217</v>
@@ -9848,7 +10488,7 @@
     </row>
     <row r="32">
       <c r="F32" t="s">
-        <v>492</v>
+        <v>63</v>
       </c>
       <c r="H32" t="s">
         <v>276</v>
@@ -9859,7 +10499,7 @@
     </row>
     <row r="33">
       <c r="F33" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H33" t="s">
         <v>286</v>
@@ -9870,7 +10510,7 @@
     </row>
     <row r="34">
       <c r="F34" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H34" t="s">
         <v>555</v>
@@ -9881,7 +10521,7 @@
     </row>
     <row r="35">
       <c r="F35" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H35" t="s">
         <v>261</v>
@@ -9892,7 +10532,7 @@
     </row>
     <row r="36">
       <c r="F36" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H36" t="s">
         <v>331</v>
@@ -9903,7 +10543,7 @@
     </row>
     <row r="37">
       <c r="F37" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H37" t="s">
         <v>308</v>
@@ -9914,7 +10554,7 @@
     </row>
     <row r="38">
       <c r="F38" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H38" t="s">
         <v>262</v>
@@ -9925,7 +10565,7 @@
     </row>
     <row r="39">
       <c r="F39" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H39" t="s">
         <v>309</v>
@@ -9935,9 +10575,6 @@
       </c>
     </row>
     <row r="40">
-      <c r="F40" t="s">
-        <v>70</v>
-      </c>
       <c r="H40" t="s">
         <v>268</v>
       </c>
@@ -10411,186 +11048,196 @@
     </row>
     <row r="99">
       <c r="Z99" t="s">
-        <v>513</v>
+        <v>636</v>
       </c>
     </row>
     <row r="100">
       <c r="Z100" t="s">
-        <v>205</v>
+        <v>637</v>
       </c>
     </row>
     <row r="101">
       <c r="Z101" t="s">
-        <v>206</v>
+        <v>513</v>
       </c>
     </row>
     <row r="102">
       <c r="Z102" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="103">
       <c r="Z103" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="104">
       <c r="Z104" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
     </row>
     <row r="105">
       <c r="Z105" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="106">
       <c r="Z106" t="s">
-        <v>575</v>
+        <v>224</v>
       </c>
     </row>
     <row r="107">
       <c r="Z107" t="s">
-        <v>627</v>
+        <v>209</v>
       </c>
     </row>
     <row r="108">
       <c r="Z108" t="s">
-        <v>593</v>
+        <v>575</v>
       </c>
     </row>
     <row r="109">
       <c r="Z109" t="s">
-        <v>149</v>
+        <v>627</v>
       </c>
     </row>
     <row r="110">
       <c r="Z110" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="111">
       <c r="Z111" t="s">
-        <v>384</v>
+        <v>149</v>
       </c>
     </row>
     <row r="112">
       <c r="Z112" t="s">
-        <v>150</v>
+        <v>594</v>
       </c>
     </row>
     <row r="113">
       <c r="Z113" t="s">
-        <v>151</v>
+        <v>384</v>
       </c>
     </row>
     <row r="114">
       <c r="Z114" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="115">
       <c r="Z115" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="116">
       <c r="Z116" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="117">
       <c r="Z117" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="118">
       <c r="Z118" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="119">
       <c r="Z119" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="120">
       <c r="Z120" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="121">
       <c r="Z121" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="122">
       <c r="Z122" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="123">
       <c r="Z123" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="124">
       <c r="Z124" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="125">
       <c r="Z125" t="s">
-        <v>514</v>
+        <v>161</v>
       </c>
     </row>
     <row r="126">
       <c r="Z126" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="127">
       <c r="Z127" t="s">
-        <v>628</v>
+        <v>514</v>
       </c>
     </row>
     <row r="128">
       <c r="Z128" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="129">
       <c r="Z129" t="s">
-        <v>165</v>
+        <v>628</v>
       </c>
     </row>
     <row r="130">
       <c r="Z130" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="131">
       <c r="Z131" t="s">
-        <v>47</v>
+        <v>165</v>
       </c>
     </row>
     <row r="132">
       <c r="Z132" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="133">
       <c r="Z133" t="s">
-        <v>168</v>
+        <v>47</v>
       </c>
     </row>
     <row r="134">
       <c r="Z134" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="135">
       <c r="Z135" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="Z136" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="Z137" t="s">
         <v>170</v>
       </c>
     </row>

</xml_diff>